<commit_message>
updated default ui spec and identity schema for eng, ara, and fra.
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/ui_spec.xlsx
+++ b/mosip_master/xlsx/ui_spec.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MOSIP\SourceCode\mayuradesh\mosip-data\lts\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Develop_Branch_all\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6294F3-D9EF-448E-BCE3-E66EB2C94300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="58">
   <si>
     <t>id</t>
   </si>
@@ -76,16 +75,7 @@
     <t>del_dtimes</t>
   </si>
   <si>
-    <t>619e3392-a37a-4476-934b-2bb4c45850bf</t>
-  </si>
-  <si>
     <t>pre-registration</t>
-  </si>
-  <si>
-    <t>Pre-Registration UI Specification</t>
-  </si>
-  <si>
-    <t>Pre-Registration UI Specification for Data Capture</t>
   </si>
   <si>
     <t>schema</t>
@@ -98,9 +88,6 @@
   </si>
   <si>
     <t>t</t>
-  </si>
-  <si>
-    <t>service-account-mosip-prereg-client</t>
   </si>
   <si>
     <t>f</t>
@@ -121,15 +108,6 @@
     <t>settings</t>
   </si>
   <si>
-    <t>[{"name":"scheduledjobs","description":{"fra":"Paramètres des travaux planifiés","eng":"Scheduled Jobs Settings"},"label":{"fra":"Paramètres des travaux planifiés","eng":"Scheduled Jobs Settings"},"fxml":"ScheduledJobsSettings.fxml","icon":"scheduledjobs.png","order":"1","shortcut-icon":"scheduledjobs-shortcut.png","access-control":["REGISTRATION_SUPERVISOR"]},{"name":"globalconfigs","description":{"fra":"Paramètres de configuration globale","eng":"Global Config Settings"},"label":{"fra":"Paramètres de configuration globale","eng":"Global Config Settings"},"fxml":"GlobalConfigSettings.fxml","icon":"globalconfigs.png","order":"2","shortcut-icon":"globalconfigs-shortcut.png","access-control":["REGISTRATION_SUPERVISOR","REGISTRATION_OFFICER"]},{"name":"devices","description":{"fra":"Réglages de l'appareil","eng":"Device Settings"},"label":{"fra":"Réglages de l'appareil","eng":"Device Settings"},"fxml":"DeviceSettings.fxml","icon":"devices.png","order":"3","shortcut-icon":"devices-shortcut.png","access-control":["REGISTRATION_SUPERVISOR","REGISTRATION_OFFICER"]}]</t>
-  </si>
-  <si>
-    <t>110024</t>
-  </si>
-  <si>
-    <t>110005</t>
-  </si>
-  <si>
     <t>0b1177a3-0e92-4f53-9176-aca49d662328</t>
   </si>
   <si>
@@ -139,79 +117,88 @@
     <t>screens</t>
   </si>
   <si>
-    <t>[{"order":1,"name":"ConsentDetails","label":{"fra":"Consentement","eng":"Consent"},"caption":{"fra":"Consentement","eng":"Consent"},"fields":["consentText","consent"],"layoutTemplate":null,"preRegFetchRequired":false,"active":false},{"order":2,"name":"DemographicDetails","label":{"fra":"Détails démographiques","eng":"Demographic Details"},"caption":{"fra":"Détails démographiques","eng":"Demographic Details"},"fields":["fullName","dateOfBirth","gender","residenceStatus","addressLine1","addressLine2","addressLine3","referenceIdentityNumber","region","province","city","zone","postalCode","phone","email","introducerName","introducerRID","introducerUIN"],"layoutTemplate":null,"preRegFetchRequired":true,"active":false},{"order":3,"name":"DocumentsDetails","label":{"fra":"Des documents","eng":"Document Upload"},"caption":{"fra":"Des documents","eng":"Documents"},"fields":["proofOfAddress","proofOfIdentity","proofOfRelationship","proofOfDateOfBirth","proofOfException","proofOfException-1"],"layoutTemplate":null,"preRegFetchRequired":false,"active":false},{"order":4,"name":"BiometricDetails","label":{"fra":"Détails biométriques","eng":"Biometric Details"},"caption":{"fra":"Détails biométriques","eng":"Biometric Details"},"fields":["individualBiometrics","individualAuthBiometrics","introducerBiometrics"],"layoutTemplate":null,"preRegFetchRequired":false,"active":false}]</t>
-  </si>
-  <si>
     <t>ff8df956-f529-45b6-9242-abe61bb02df9</t>
   </si>
   <si>
     <t>Fields spec</t>
   </si>
   <si>
-    <t>Field spec</t>
-  </si>
-  <si>
-    <t>[{"id":"IDSchemaVersion","inputRequired":false,"type":"number","minimum":0,"maximum":0,"description":"ID Schema Version","label":{"eng":"IDSchemaVersion"},"controlType":null,"fieldType":"default","format":"none","validators":[],"fieldCategory":"none","alignmentGroup":null,"visible":null,"contactType":null,"group":null,"groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"IdSchemaVersion"},{"id":"UIN","inputRequired":false,"type":"string","minimum":0,"maximum":0,"description":"UIN","label":{"eng":"UIN"},"controlType":"textbox","fieldType":"default","format":"none","validators":[],"fieldCategory":"none","alignmentGroup":null,"visible":null,"contactType":null,"group":null,"groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"UIN"},{"id":"fullName","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"Full Name","label":{"fra":"Nom complet","eng":"Full Name"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"FullName","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"name"},{"id":"dateOfBirth","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"dateOfBirth","label":{"fra":"DOB","eng":"DOB"},"controlType":"ageDate","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])/([0][1-9]|1[0-2])/([0][1-9]|[1-2][0-9]|3[01])$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"DateOfBirth","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.isNew || (identity.isUpdate &amp;&amp; (identity.updatableFieldGroups contains 'IntroducerDetails' || identity.updatableFieldGroups contains 'DateOfBirth'))"}],"subType":"dateOfBirth"},{"id":"gender","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"gender","label":{"fra":"Le genre","eng":"Gender"},"controlType":"dropdown","fieldType":"dynamic","format":"","validators":[],"fieldCategory":"pvt","alignmentGroup":"group1","visible":null,"contactType":null,"group":"Gender","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"gender"},{"id":"addressLine1","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine1","label":{"fra":"line1","eng":"line1"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"addressLine1"},{"id":"addressLine2","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine2","label":{"fra":"line2","eng":"line2"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"addressLine2"},{"id":"addressLine3","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine3","label":{"fra":"line3","eng":"line3"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"addressLine3"},{"id":"residenceStatus","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"residenceStatus","label":{"fra":"Reside Status","eng":"Residence Status"},"controlType":"dropdown","fieldType":"dynamic","format":"none","validators":[],"fieldCategory":"kyc","alignmentGroup":"group1","visible":null,"contactType":null,"group":"ResidenceStatus","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"residenceStatus"},{"id":"referenceIdentityNumber","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"referenceIdentityNumber","label":{"fra":"Reference Identity Number","eng":"Reference Identity Number"},"controlType":"textbox","fieldType":"default","format":"kyc","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"ReferenceIdentityNumber","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"none"},{"id":"region","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"region","label":{"fra":"Region","eng":"Region"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Region"},{"id":"province","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"province","label":{"fra":"Province","eng":"Province"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Province"},{"id":"city","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"city","label":{"fra":"City","eng":"City"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"City"},{"id":"zone","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"zone","label":{"fra":"Zone","eng":"Zone"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":null,"group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Zone"},{"id":"postalCode","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"postalCode","label":{"fra":"Postal","eng":"Postal"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[(?i)A-Z0-9]{5}$|^NA$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Postal Code"},{"id":"phone","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"phone","label":{"fra":"Phone","eng":"Phone"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[+]*([0-9]{1})([0-9]{9})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"contact","visible":null,"contactType":"email","group":"Phone","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Phone"},{"id":"email","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"email","label":{"fra":"Email","eng":"Email"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[A-Za-z0-9_\\-]+(\\.[A-Za-z0-9_]+)*@[A-Za-z0-9_-]+(\\.[A-Za-z0-9_]+)*(\\.[a-zA-Z]{2,})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"contact","visible":null,"contactType":"email","group":"Email","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Email"},{"id":"introducerName","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"introducerName","label":{"fra":"nom del'introducteur","eng":"Introducer Name"},"controlType":"textbox","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":null,"contactType":null,"group":"IntroducerDetails","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"( identity.isNew &amp;&amp; identity.isChild ) || ( identity.isUpdate &amp;&amp; identity.isChild ) || ( !(identity.get('introducerRID') == nil || identity.get('introducerRID') == empty) ||   !(identity.get('introducerUIN') == nil || identity.get('introducerUIN') == empty))"}],"subType":"introducerName"},{"id":"introducerRID","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"introducerRID","label":{"fra":"Introducteur RID","eng":"Introducer RID"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":null,"contactType":null,"group":"IntroducerDetails","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"( !(identity.get('introducerName') == nil || identity.get('introducerName') == empty) &amp;&amp;   (identity.get('introducerUIN') == nil || identity.get('introducerUIN') == empty))"}],"subType":"RID"},{"id":"introducerUIN","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"introducerUIN","label":{"fra":"Introducteur UIN","eng":"Introducer UIN"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":null,"contactType":null,"group":"IntroducerDetails","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"( !(identity.get('introducerName') == nil || identity.get('introducerName') == empty) &amp;&amp;   (identity.get('introducerRID') == nil || identity.get('introducerRID') == empty))"}],"subType":"UIN"},{"id":"proofOfAddress","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfAddress","label":{"fra":"Address Proof","eng":"Address Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.isNew || ( identity.isUpdate &amp;&amp; (identity.updatableFields contains 'addressLine1' || identity.updatableFields contains 'addressLine2' || identity.updatableFields contains 'addressLine3'))"}],"subType":"POA"},{"id":"proofOfIdentity","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfIdentity","label":{"fra":"Identity Proof","eng":"Identity Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.isNew || ( identity.isUpdate &amp;&amp; identity.updatableFields contains 'fullName')"}],"subType":"POI"},{"id":"proofOfRelationship","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfRelationship","label":{"fra":"Relationship Proof","eng":"Relationship Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"( identity.isNew &amp;&amp; identity.isChild ) || ( identity.isUpdate &amp;&amp; (identity.updatableFieldGroups contains 'IntroducerDetails' || identity.isChild))"}],"subType":"POR"},{"id":"proofOfDateOfBirth","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfDateOfBirth","label":{"fra":"DOB Proof","eng":"DOB Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.isUpdate &amp;&amp; identity.updatableFields contains 'dateOfBirth'"}],"subType":"POB"},{"id":"proofOfException","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfException","label":{"fra":"Exception Proof","eng":"Exception Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"POE"},{"id":"proofOfException-1","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfException","label":{"fra":"Exception Proof","eng":"Exception Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"POE"},{"id":"individualBiometrics","inputRequired":true,"type":"biometricsType","minimum":0,"maximum":0,"description":"","label":{"fra":"Applicant Biometrics","eng":"Applicant Biometrics"},"controlType":"biometrics","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Biometrics","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"requiredOn":[{"engine":"MVEL","expr":"(identity.isNew || identity.isLost || ( identity.isUpdate &amp;&amp; identity.updatableFieldGroups contains 'Biometrics'))"}],"subType":"applicant"},{"id":"individualAuthBiometrics","inputRequired":true,"type":"biometricsType","minimum":0,"maximum":0,"description":"Used to hold biometrics only for authentication","label":{"fra":"Authentication Biometrics","eng":"Authentication Biometrics"},"controlType":"biometrics","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":null,"groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"requiredOn":[{"engine":"MVEL","expr":"!identity.isChild &amp;&amp; identity.isUpdate &amp;&amp; !(identity.updatableFieldGroups contains 'Biometrics' || identity.updatableFieldGroups contains 'IntroducerDetails')"}],"subType":"applicant-auth"},{"id":"introducerBiometrics","inputRequired":true,"type":"biometricsType","minimum":0,"maximum":0,"description":"","label":{"fra":"Introducteur Biométrie","eng":"Introducer Biometrics"},"controlType":"biometrics","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Biometrics","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"requiredOn":[{"engine":"MVEL","expr":"(identity.isChild &amp;&amp; identity.isNew) || (identity.isUpdate &amp;&amp; identity.updatableFieldGroups contains 'IntroducerDetails') || !(identity.get('introducerName') == nil || identity.get('introducerName') == empty)"}],"subType":"introducer"},{"id":"consentText","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"Consent","label":{},"controlType":"html","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"consentText","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":"Registration Consent","fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"consentText"},{"id":"consent","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"consent accepted","label":{"fra":"J'ai lu et j'accepte les termes et conditions pour partager mes PII","eng":"I have read and accept terms and conditions to share my PII"},"controlType":"checkbox","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"consent","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"consent"}]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c1ef9f1c-b1b6-4c78-871f-000ed543c191 </t>
-  </si>
-  <si>
-    <t>New registration process</t>
-  </si>
-  <si>
     <t>newProcess</t>
-  </si>
-  <si>
-    <t>{"id":"NEW","order":1,"flow":"NEW","isSubProcess":false,"label":{"eng":"New Registration","fra":"Nouvelle inscription"},"screens":[{"order":1,"name":"consentdet","label":{"fra":"Consentement","eng":"Consent"},"caption":{"fra":"Consentement","eng":"Consent"},"fields":[{"id":"IDSchemaVersion","inputRequired":false,"type":"number","minimum":0,"maximum":0,"description":"ID Schema Version","label":{"eng":"IDSchemaVersion"},"controlType":null,"fieldType":"default","format":"none","validators":[],"fieldCategory":"none","alignmentGroup":null,"visible":null,"contactType":null,"group":null,"groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"IdSchemaVersion"},{"id":"consentText","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"Consent","label":{},"controlType":"html","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"consentText","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":"Registration Consent","fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"consentText"},{"id":"consent","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"consent accepted","label":{"fra":"J'ai lu et j'accepte les termes et conditions pour partager mes PII","eng":"I have read and accept terms and conditions to share my PII"},"controlType":"checkbox","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"consent","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"consent"},{"id":"preferredLang","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"user preferred Language","label":{"fra":"Langue de notification","eng":"Notification Langauge"},"controlType":"button","fieldType":"dynamic","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":"group1","visible":null,"contactType":null,"group":"PreferredLanguage","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"preferredLang"}],"layoutTemplate":null,"preRegFetchRequired":false,"active":false},{"order":2,"name":"DemographicDetails","label":{"fra":"Détails démographiques","eng":"Demographic Details"},"caption":{"fra":"Détails démographiques","eng":"Demographic Details"},"fields":[{"id":"fullName","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"Full Name","label":{"fra":"Nom complet","eng":"Full Name"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"FullName","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"name"},{"id":"dateOfBirth","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"dateOfBirth","label":{"fra":"DOB","eng":"DOB"},"controlType":"ageDate","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])/([0][1-9]|1[0-2])/([0][1-9]|[1-2][0-9]|3[01])$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"DateOfBirth","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"dateOfBirth"},{"id":"gender","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"gender","label":{"fra":"Le genre","eng":"Gender"},"controlType":"button","fieldType":"dynamic","format":"","validators":[],"fieldCategory":"pvt","alignmentGroup":"group1","visible":null,"contactType":null,"group":"Gender","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"gender"},{"id":"addressLine1","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine1","label":{"fra":"line1","eng":"line1"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"addressLine1"},{"id":"addressLine2","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine2","label":{"fra":"line2","eng":"line2"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"addressLine2"},{"id":"addressLine3","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine3","label":{"fra":"line3","eng":"line3"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"addressLine3"},{"id":"residenceStatus","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"residenceStatus","label":{"fra":"Reside Status","eng":"Residence Status"},"controlType":"button","fieldType":"dynamic","format":"none","validators":[],"fieldCategory":"kyc","alignmentGroup":"group1","visible":null,"contactType":null,"group":"ResidenceStatus","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"residenceStatus"},{"id":"referenceIdentityNumber","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"referenceIdentityNumber","label":{"fra":"Reference Identity Number","eng":"Reference Identity Number"},"controlType":"textbox","fieldType":"default","format":"kyc","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"ReferenceIdentityNumber","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"none"},{"id":"region","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"region","label":{"fra":"Region","eng":"Region"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Region"},{"id":"province","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"province","label":{"fra":"Province","eng":"Province"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Province"},{"id":"city","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"city","label":{"fra":"City","eng":"City"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"City"},{"id":"zone","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"zone","label":{"fra":"Zone","eng":"Zone"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":null,"group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Zone"},{"id":"postalCode","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"postalCode","label":{"fra":"Postal","eng":"Postal"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[(?i)A-Z0-9]{5}$|^NA$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Postal Code"},{"id":"phone","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"phone","label":{"fra":"Phone","eng":"Phone"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[+]*([0-9]{1})([0-9]{9})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"contact","visible":null,"contactType":"email","group":"Phone","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Phone"},{"id":"email","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"email","label":{"fra":"Email","eng":"Email"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[A-Za-z0-9_\\-]+(\\.[A-Za-z0-9_]+)*@[A-Za-z0-9_-]+(\\.[A-Za-z0-9_]+)*(\\.[a-zA-Z]{2,})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"contact","visible":null,"contactType":"email","group":"Email","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Email"},{"id":"introducerName","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"introducerName","label":{"fra":"nom del'introducteur","eng":"Introducer Name"},"controlType":"textbox","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT'"},"contactType":null,"group":"IntroducerDetails","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT'"}],"subType":"introducerName"},{"id":"introducerRID","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"introducerRID","label":{"fra":"Introducteur RID","eng":"Introducer RID"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT' &amp;&amp; (identity.get('introducerUIN') == nil || identity.get('introducerUIN') == empty)"},"contactType":null,"group":"IntroducerDetails","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT' &amp;&amp; (identity.get('introducerUIN') == nil || identity.get('introducerUIN') == empty)"}],"subType":"RID"},{"id":"introducerUIN","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"introducerUIN","label":{"fra":"Introducteur UIN","eng":"Introducer UIN"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT' &amp;&amp; (identity.get('introducerRID') == nil || identity.get('introducerRID') == empty)"},"contactType":null,"group":"IntroducerDetails","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT' &amp;&amp; (identity.get('introducerRID') == nil || identity.get('introducerRID') == empty)"}],"subType":"UIN"}],"layoutTemplate":null,"preRegFetchRequired":true,"active":false},{"order":3,"name":"Documents","label":{"fra":"Des documents","eng":"Document Upload"},"caption":{"fra":"Des documents","eng":"Documents"},"fields":[{"id":"proofOfAddress","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfAddress","label":{"fra":"Address Proof","eng":"Address Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"POA"},{"id":"proofOfIdentity","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfIdentity","label":{"fra":"Identity Proof","eng":"Identity Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"POI"},{"id":"proofOfRelationship","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfRelationship","label":{"fra":"Relationship Proof","eng":"Relationship Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT'"}],"subType":"POR"},{"id":"proofOfDateOfBirth","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfDateOfBirth","label":{"fra":"DOB Proof","eng":"DOB Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"POB"},{"id":"proofOfException","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfException","label":{"fra":"Exception Proof","eng":"Exception Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"POE"}],"layoutTemplate":null,"preRegFetchRequired":false,"active":false},{"order":4,"name":"BiometricDetails","label":{"fra":"Détails biométriques","eng":"Biometric Details"},"caption":{"fra":"Détails biométriques","eng":"Biometric Details"},"fields":[{"id":"individualBiometrics","inputRequired":true,"type":"biometricsType","minimum":0,"maximum":0,"description":"","label":{"fra":"Applicant Biometrics","eng":"Applicant Biometrics"},"controlType":"biometrics","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Biometrics","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":[{"ageGroup":"INFANT","process":"ALL","validationExpr":"face","bioAttributes":["face"]}],"required":true,"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"requiredOn":[],"subType":"applicant"},{"id":"introducerBiometrics","inputRequired":true,"type":"biometricsType","minimum":0,"maximum":0,"description":"","label":{"fra":"Introducteur Biométrie","eng":"Introducer Biometrics"},"controlType":"biometrics","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Biometrics","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":[{"ageGroup":"INFANT","process":"ALL","validationExpr":"leftEye || rightEye || rightIndex || rightLittle || rightRing || rightMiddle || leftIndex || leftLittle || leftRing || leftMiddle || leftThumb || rightThumb || face","bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"]}],"required":false,"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"requiredOn":[{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT'"}],"subType":"introducer"}],"layoutTemplate":null,"preRegFetchRequired":false,"active":false}],"caption":{"eng":"New Registration","fra":"Nouvelle inscription"},"icon":"NewReg.png","isActive":true,"autoSelectedGroups":null}</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">703796d8-085f-4778-80be-df298c1b8367 </t>
-  </si>
-  <si>
-    <t>Update registration process</t>
   </si>
   <si>
     <t>updateProcess</t>
   </si>
   <si>
-    <t>{"id":"UPDATE","order":2,"flow":"UPDATE","isSubProcess":false,"label":{"eng":"Update UIN","fra":"Mettre à jour l'UIN"},"screens":[{"order":1,"name":"consentdet","label":{"fra":"Consentement","eng":"Consent"},"caption":{"fra":"Consentement","eng":"Consent"},"fields":[{"id":"consentText","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"Consent","label":{},"controlType":"html","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"Consent","groupLabel":{"fra":"Consentement","eng":"Consent"},"changeAction":null,"transliterate":false,"templateName":"Registration Consent","fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"consentText"},{"id":"consent","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"consent accepted","label":{"fra":"J'ai lu et j'accepte les termes et conditions pour partager mes PII","eng":"I have read and accept terms and conditions to share my PII"},"controlType":"checkbox","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"Consent","groupLabel":{"fra":"Consentement","eng":"Consent"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"consent"},{"id":"preferredLang","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"user preferred Language","label":{"fra":"Langue de notification","eng":"Notification Langauge"},"controlType":"button","fieldType":"dynamic","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":"group1","visible":null,"contactType":null,"group":"PreferredLanguage","groupLabel":{"fra":"Langue de notification","eng":"Notification Langauge"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"preferredLang"}],"layoutTemplate":null,"preRegFetchRequired":false,"active":false},{"order":2,"name":"DemographicDetails","label":{"fra":"Détails démographiques","eng":"Demographic Details"},"caption":{"fra":"Détails démographiques","eng":"Demographic Details"},"fields":[{"id":"fullName","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"Full Name","label":{"fra":"Nom complet","eng":"Full Name"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"FullName","groupLabel":{"fra":"Nom complet","eng":"Full Name"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"name"},{"id":"dateOfBirth","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"dateOfBirth","label":{"fra":"DOB","eng":"DOB"},"controlType":"ageDate","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])/([0][1-9]|1[0-2])/([0][1-9]|[1-2][0-9]|3[01])$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"DateOfBirth","groupLabel":{"fra":"Date de naissance","eng":"Date Of Birth"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"dateOfBirth"},{"id":"gender","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"gender","label":{"fra":"Le genre","eng":"Gender"},"controlType":"button","fieldType":"dynamic","format":"","validators":[],"fieldCategory":"pvt","alignmentGroup":"group1","visible":null,"contactType":null,"group":"Gender","groupLabel":{"fra":"Le genre","eng":"Gender"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"gender"},{"id":"addressLine1","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine1","label":{"fra":"line1","eng":"line1"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":{"fra":"Adresse","eng":"Address"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"addressLine1"},{"id":"addressLine2","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine2","label":{"fra":"line2","eng":"line2"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":{"fra":"Adresse","eng":"Address"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"addressLine2"},{"id":"addressLine3","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine3","label":{"fra":"line3","eng":"line3"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":{"fra":"Adresse","eng":"Address"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"addressLine3"},{"id":"residenceStatus","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"residenceStatus","label":{"fra":"Reside Status","eng":"Residence Status"},"controlType":"button","fieldType":"dynamic","format":"none","validators":[],"fieldCategory":"kyc","alignmentGroup":"group1","visible":null,"contactType":null,"group":"ResidenceStatus","groupLabel":{"fra":"Reside Status","eng":"Residence Status"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"residenceStatus"},{"id":"referenceIdentityNumber","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"referenceIdentityNumber","label":{"fra":"Reference Identity Number","eng":"Reference Identity Number"},"controlType":"textbox","fieldType":"default","format":"kyc","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"ReferenceIdentityNumber","groupLabel":{"fra":"Reference Identity Number","eng":"Reference Identity Number"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"none"},{"id":"region","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"region","label":{"fra":"Region","eng":"Region"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":{"fra":"Lieu","eng":"Location"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Region"},{"id":"province","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"province","label":{"fra":"Province","eng":"Province"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":{"fra":"Lieu","eng":"Location"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Province"},{"id":"city","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"city","label":{"fra":"City","eng":"City"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":{"fra":"Lieu","eng":"Location"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"City"},{"id":"zone","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"zone","label":{"fra":"Zone","eng":"Zone"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":null,"group":"Location","groupLabel":{"fra":"Lieu","eng":"Location"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Zone"},{"id":"postalCode","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"postalCode","label":{"fra":"Postal","eng":"Postal"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[(?i)A-Z0-9]{5}$|^NA$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":{"fra":"Lieu","eng":"Location"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Postal Code"},{"id":"phone","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"phone","label":{"fra":"Phone","eng":"Phone"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[+]*([0-9]{1})([0-9]{9})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"contact","visible":null,"contactType":"email","group":"Phone","groupLabel":{"fra":"Phone","eng":"Phone"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Phone"},{"id":"email","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"email","label":{"fra":"Email","eng":"Email"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[A-Za-z0-9_\\-]+(\\.[A-Za-z0-9_]+)*@[A-Za-z0-9_-]+(\\.[A-Za-z0-9_]+)*(\\.[a-zA-Z]{2,})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"contact","visible":null,"contactType":"email","group":"Email","groupLabel":{"fra":"Email","eng":"Email"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Email"},{"id":"introducerName","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"introducerName","label":{"fra":"nom del'introducteur","eng":"Introducer Name"},"controlType":"textbox","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":null,"contactType":null,"group":"IntroducerDetails","groupLabel":{"eng":"Introducer Details","fra":"Détails de l'introducteur"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"introducerName"},{"id":"introducerRID","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"introducerRID","label":{"fra":"Introducteur RID","eng":"Introducer RID"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":{"engine":"MVEL","expr":"identity.get('introducerUIN') == nil || identity.get('introducerUIN') == empty"},"contactType":null,"group":"IntroducerDetails","groupLabel":{"eng":"Introducer Details","fra":"Détails de l'introducteur"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.get('introducerUIN') == nil || identity.get('introducerUIN') == empty"}],"subType":"RID"},{"id":"introducerUIN","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"introducerUIN","label":{"fra":"Introducteur UIN","eng":"Introducer UIN"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":{"engine":"MVEL","expr":"identity.get('introducerRID') == nil || identity.get('introducerRID') == empty"},"contactType":null,"group":"IntroducerDetails","groupLabel":{"eng":"Introducer Details","fra":"Détails de l'introducteur"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.get('introducerRID') == nil || identity.get('introducerRID') == empty"}],"subType":"UIN"}],"layoutTemplate":null,"preRegFetchRequired":true,"active":false},{"order":3,"name":"Documents","label":{"fra":"Des documents","eng":"Document Upload"},"caption":{"fra":"Des documents","eng":"Documents"},"fields":[{"id":"proofOfAddress","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfAddress","label":{"fra":"Address Proof","eng":"Address Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":{"fra":"Documents","eng":"Documents"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.updatableFieldGroups contains 'Address' || identity.updatableFieldGroups contains 'Location'"}],"subType":"POA"},{"id":"proofOfIdentity","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfIdentity","label":{"fra":"Identity Proof","eng":"Identity Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":{"fra":"Documents","eng":"Documents"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.updatableFieldGroups contains 'FullName' || identity.updatableFieldGroups contains 'DateOfBirth'"}],"subType":"POI"},{"id":"proofOfRelationship","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfRelationship","label":{"fra":"Relationship Proof","eng":"Relationship Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":{"fra":"Documents","eng":"Documents"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT' || identity.updatableFieldGroups contains 'IntroducerDetails'"}],"subType":"POR"},{"id":"proofOfDateOfBirth","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfDateOfBirth","label":{"fra":"DOB Proof","eng":"DOB Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":{"fra":"Documents","eng":"Documents"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.updatableFieldGroups contains 'DateOfBirth'"}],"subType":"POB"},{"id":"proofOfException","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfException","label":{"fra":"Exception Proof","eng":"Exception Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":{"fra":"Documents","eng":"Documents"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"POE"}],"layoutTemplate":null,"preRegFetchRequired":false,"active":false},{"order":4,"name":"BiometricDetails","label":{"fra":"Détails biométriques","eng":"Biometric Details"},"caption":{"fra":"Détails biométriques","eng":"Biometric Details"},"fields":[{"id":"individualBiometrics","inputRequired":true,"type":"biometricsType","minimum":0,"maximum":0,"description":"","label":{"fra":"Biométrie du demandeur","eng":"Applicant Biometrics"},"controlType":"biometrics","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Biometrics","groupLabel":{"fra":"Biométrie","eng":"Biometrics"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":[{"ageGroup":"INFANT","process":"ALL","validationExpr":"face","bioAttributes":["face"]}],"required":true,"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"requiredOn":[{"engine":"MVEL","expr":"identity.updatableFieldGroups contains 'Biometrics'"}],"subType":"applicant"},{"id":"individualAuthBiometrics","inputRequired":true,"type":"biometricsType","minimum":0,"maximum":0,"description":"Used to hold biometrics only for authentication","label":{"fra":"Authentification Biométrie","eng":"Authentication Biometrics"},"controlType":"biometrics","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Biometrics","groupLabel":{"fra":"Biométrie","eng":"Biometrics"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":[{"ageGroup":"ALL","process":"ALL","validationExpr":"leftEye || rightEye || rightIndex || rightLittle || rightRing || rightMiddle || leftIndex || leftLittle || leftRing || leftMiddle || leftThumb || rightThumb || face","bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"]}],"required":false,"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"requiredOn":[{"engine":"MVEL","expr":"!(identity.get('ageGroup') == 'INFANT') &amp;&amp; !(identity.updatableFieldGroups contains 'Biometrics')"}],"subType":"applicant-auth"},{"id":"introducerBiometrics","inputRequired":true,"type":"biometricsType","minimum":0,"maximum":0,"description":"","label":{"fra":"Introducteur Biométrie","eng":"Introducer Biometrics"},"controlType":"biometrics","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Biometrics","groupLabel":{"fra":"Biométrie","eng":"Biometrics"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":[{"ageGroup":"ALL","process":"ALL","validationExpr":"leftEye || rightEye || rightIndex || rightLittle || rightRing || rightMiddle || leftIndex || leftLittle || leftRing || leftMiddle || leftThumb || rightThumb || face","bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"]}],"required":false,"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"requiredOn":[{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT' || identity.updatableFieldGroups contains 'IntroducerDetails'"}],"subType":"introducer"}],"layoutTemplate":null,"preRegFetchRequired":false,"active":false}],"caption":{"eng":"Update UIN","fra":"Mettre à jour l'UIN"},"icon":"UINUpdate.png","isActive":true,"autoSelectedGroups":["Consent","PreferredLanguage","Documents","Biometrics"]}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78f07cba-0f5d-4e28-a970-f85d1ac302c9 </t>
-  </si>
-  <si>
-    <t>Lost registration process</t>
-  </si>
-  <si>
     <t>lostProcess</t>
-  </si>
-  <si>
-    <t>{"id":"LOST","order":3,"flow":"LOST","isSubProcess":false,"label":{"eng":"Lost UIN","fra":"UIN perdu"},"screens":[{"order":1,"name":"consentdet","label":{"fra":"Consentement","eng":"Consent"},"caption":{"fra":"Consentement","eng":"Consent"},"fields":[{"id":"IDSchemaVersion","inputRequired":false,"type":"number","minimum":0,"maximum":0,"description":"ID Schema Version","label":{"eng":"IDSchemaVersion"},"controlType":null,"fieldType":"default","format":"none","validators":[],"fieldCategory":"none","alignmentGroup":null,"visible":null,"contactType":null,"group":null,"groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"IdSchemaVersion"},{"id":"consentText","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"Consent","label":{},"controlType":"html","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"consentText","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":"Registration Consent","fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"consentText"},{"id":"consent","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"consent accepted","label":{"fra":"J'ai lu et j'accepte les termes et conditions pour partager mes PII","eng":"I have read and accept terms and conditions to share my PII"},"controlType":"checkbox","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"consent","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"consent"},{"id":"preferredLang","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"user preferred Language","label":{"fra":"Langue de notification","eng":"Notification Langauge"},"controlType":"button","fieldType":"dynamic","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":"group1","visible":null,"contactType":null,"group":"PreferredLanguage","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"preferredLang"}],"layoutTemplate":null,"preRegFetchRequired":false,"active":false},{"order":2,"name":"DemographicDetails","label":{"fra":"Détails démographiques","eng":"Demographic Details"},"caption":{"fra":"Détails démographiques","eng":"Demographic Details"},"fields":[{"id":"fullName","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"Full Name","label":{"fra":"Nom complet","eng":"Full Name"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"FullName","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"name"},{"id":"dateOfBirth","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"dateOfBirth","label":{"fra":"DOB","eng":"DOB"},"controlType":"ageDate","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])/([0][1-9]|1[0-2])/([0][1-9]|[1-2][0-9]|3[01])$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"DateOfBirth","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"dateOfBirth"},{"id":"gender","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"gender","label":{"fra":"Le genre","eng":"Gender"},"controlType":"button","fieldType":"dynamic","format":"","validators":[],"fieldCategory":"pvt","alignmentGroup":"group1","visible":null,"contactType":null,"group":"Gender","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"gender"},{"id":"addressLine1","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine1","label":{"fra":"line1","eng":"line1"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"addressLine1"},{"id":"addressLine2","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine2","label":{"fra":"line2","eng":"line2"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"addressLine2"},{"id":"addressLine3","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine3","label":{"fra":"line3","eng":"line3"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"addressLine3"},{"id":"residenceStatus","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"residenceStatus","label":{"fra":"Reside Status","eng":"Residence Status"},"controlType":"button","fieldType":"dynamic","format":"none","validators":[],"fieldCategory":"kyc","alignmentGroup":"group1","visible":null,"contactType":null,"group":"ResidenceStatus","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"residenceStatus"},{"id":"referenceIdentityNumber","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"referenceIdentityNumber","label":{"fra":"Reference Identity Number","eng":"Reference Identity Number"},"controlType":"textbox","fieldType":"default","format":"kyc","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"ReferenceIdentityNumber","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"none"},{"id":"region","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"region","label":{"fra":"Region","eng":"Region"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"Region"},{"id":"province","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"province","label":{"fra":"Province","eng":"Province"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"Province"},{"id":"city","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"city","label":{"fra":"City","eng":"City"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"City"},{"id":"zone","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"zone","label":{"fra":"Zone","eng":"Zone"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":null,"group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"Zone"},{"id":"postalCode","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"postalCode","label":{"fra":"Postal","eng":"Postal"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[(?i)A-Z0-9]{5}$|^NA$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"Postal Code"},{"id":"phone","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"phone","label":{"fra":"Phone","eng":"Phone"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[+]*([0-9]{1})([0-9]{9})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"contact","visible":null,"contactType":"email","group":"Phone","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"Phone"},{"id":"email","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"email","label":{"fra":"Email","eng":"Email"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[A-Za-z0-9_\\-]+(\\.[A-Za-z0-9_]+)*@[A-Za-z0-9_-]+(\\.[A-Za-z0-9_]+)*(\\.[a-zA-Z]{2,})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"contact","visible":null,"contactType":"email","group":"Email","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"Email"},{"id":"introducerName","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"introducerName","label":{"fra":"nom del'introducteur","eng":"Introducer Name"},"controlType":"textbox","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT'"},"contactType":null,"group":"IntroducerDetails","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT'"}],"subType":"introducerName"},{"id":"introducerRID","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"introducerRID","label":{"fra":"Introducteur RID","eng":"Introducer RID"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT' &amp;&amp; (identity.get('introducerUIN') == nil || identity.get('introducerUIN') == empty)"},"contactType":null,"group":"IntroducerDetails","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT' &amp;&amp; (identity.get('introducerUIN') == nil || identity.get('introducerUIN') == empty)"}],"subType":"RID"},{"id":"introducerUIN","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"introducerUIN","label":{"fra":"Introducteur UIN","eng":"Introducer UIN"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT' &amp;&amp; (identity.get('introducerRID') == nil || identity.get('introducerRID') == empty)"},"contactType":null,"group":"IntroducerDetails","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT' &amp;&amp; (identity.get('introducerRID') == nil || identity.get('introducerRID') == empty)"}],"subType":"UIN"}],"layoutTemplate":null,"preRegFetchRequired":true,"active":false},{"order":3,"name":"BiometricDetails","label":{"fra":"Détails biométriques","eng":"Biometric Details"},"caption":{"fra":"Détails biométriques","eng":"Biometric Details"},"fields":[{"id":"individualBiometrics","inputRequired":true,"type":"biometricsType","minimum":0,"maximum":0,"description":"","label":{"fra":"Applicant Biometrics","eng":"Applicant Biometrics"},"controlType":"biometrics","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Biometrics","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":[{"ageGroup":"INFANT","process":"ALL","validationExpr":"face","bioAttributes":["face"]}],"required":true,"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"requiredOn":[],"subType":"applicant"},{"id":"proofOfException","inputRequired":false,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfException","label":{"fra":"Exception Proof","eng":"Exception Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"POE"}],"layoutTemplate":null,"preRegFetchRequired":false,"active":false}],"caption":{"eng":"Lost UIN","fra":"UIN perdu"},"icon":"LostUIN.png","isActive":true,"autoSelectedGroups":null}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6a080562-86d0-4dba-8bd9-4bdc89243e70 </t>
-  </si>
-  <si>
-    <t>Bio correction registration process</t>
   </si>
   <si>
     <t>bioCorrectionProcess</t>
   </si>
   <si>
-    <t>{"id":"BIOMETRIC_CORRECTION","order":4,"flow":"CORRECTION","isSubProcess":false,"label":{"eng":"Biometric correction","fra":"Correction biométrique"},"screens":[{"order":1,"name":"consentdet","label":{"fra":"Consentement","eng":"Consent"},"caption":{"fra":"Consentement","eng":"Consent"},"fields":[{"id":"consentText","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"Consent","label":{},"controlType":"html","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"consentText","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":"Registration Consent","fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"consentText"},{"id":"consent","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"consent accepted","label":{"fra":"J'ai lu et j'accepte les termes et conditions pour partager mes PII","eng":"I have read and accept terms and conditions to share my PII"},"controlType":"checkbox","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"consent","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"consent"},{"id":"preferredLang","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"user preferred Language","label":{"fra":"Langue de notification","eng":"Notification Langauge"},"controlType":"button","fieldType":"dynamic","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":"group1","visible":null,"contactType":null,"group":"PreferredLanguage","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"preferredLang"}],"layoutTemplate":null,"preRegFetchRequired":false,"additionalInfoRequestIdRequired":false,"active":false},{"order":2,"name":"BiometricDetails","label":{"fra":"Détails biométriques","eng":"Biometric Details"},"caption":{"fra":"Détails biométriques","eng":"Biometric Details"},"fields":[{"id":"individualBiometrics","inputRequired":true,"type":"biometricsType","minimum":0,"maximum":0,"description":"","label":{"fra":"Applicant Biometrics","eng":"Applicant Biometrics"},"controlType":"biometrics","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Biometrics","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":[{"ageGroup":"INFANT","process":"ALL","validationExpr":"face","bioAttributes":["face"]}],"required":true,"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"requiredOn":[],"subType":"applicant"},{"id":"proofOfException","inputRequired":false,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfException","label":{"fra":"Exception Proof","eng":"Exception Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"POE"}],"layoutTemplate":null,"preRegFetchRequired":false,"additionalInfoRequestIdRequired":true,"active":false}],"caption":{"eng":"Biometric correction","fra":"Correction biométrique"},"icon":"UINUpdate.png","isActive":true,"autoSelectedGroups":null}</t>
+    <t>[{"name":"scheduledjobs","description":{"ara":"إعدادات الوظائف المجدولة","fra":"Paramètres des travaux planifiés","eng":"Scheduled Jobs Settings"},"label":{"ara":"إعدادات الوظائف المجدولة","fra":"Paramètres des travaux planifiés","eng":"Scheduled Jobs Settings"},"fxml":"ScheduledJobsSettings.fxml","icon":"scheduledjobs.png","order":"1","shortcut-icon":"scheduledjobs-shortcut.png","access-control":["REGISTRATION_SUPERVISOR"]},{"name":"globalconfigs","description":{"ara":"إعدادات التكوين العامة","fra":"Paramètres de configuration globale","eng":"Global Config Settings"},"label":{"ara":"إعدادات التكوين العامة","fra":"Paramètres de configuration globale","eng":"Global Config Settings"},"fxml":"GlobalConfigSettings.fxml","icon":"globalconfigs.png","order":"2","shortcut-icon":"globalconfigs-shortcut.png","access-control":["REGISTRATION_SUPERVISOR","REGISTRATION_OFFICER"]},{"name":"devices","description":{"ara":"إعدادات الجهاز","fra":"Réglages de l'appareil","eng":"Device Settings"},"label":{"ara":"إعدادات الجهاز","fra":"Réglages de l'appareil","eng":"Device Settings"},"fxml":"DeviceSettings.fxml","icon":"devices.png","order":"3","shortcut-icon":"devices-shortcut.png","access-control":["REGISTRATION_SUPERVISOR","REGISTRATION_OFFICER"]}]</t>
   </si>
   <si>
-    <t>{"identity":{"identity":[{"id":"IDSchemaVersion","description":"ID Schema Version","type":"number","controlType":null,"fieldType":"default","inputRequired":false,"validators":[],"required":true},{"id":"fullName","description":"Enter Full Name","labelName":{"eng":"Full Name","fra":"Nom complet"},"controlType":"textbox","inputRequired":true,"fieldType":"default","type":"simpleType","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[]}],"required":true,"transliteration":true},{"id":"dateOfBirth","description":"Enter DOB","labelName":{"eng":"Date Of Birth","fra":"Date de naissance"},"controlType":"ageDate","inputRequired":true,"fieldType":"default","type":"string","validators":[],"required":true},{"id":"gender","description":"Enter Gender","labelName":{"eng":"Gender","fra":"Le genre"},"controlType":"dropdown","inputRequired":true,"fieldType":"dynamic","type":"simpleType","validators":[],"required":true},{"id":"residenceStatus","description":"Residence status","labelName":{"eng":"Residence Status","fra":"Statut de résidence"},"controlType":"dropdown","inputRequired":true,"fieldType":"dynamic","type":"simpleType","validators":[],"required":true},{"id":"addressLine1","description":"addressLine1","labelName":{"eng":"Address Line1","fra":"Adresse 1"},"controlType":"textbox","inputRequired":true,"fieldType":"default","type":"simpleType","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[]}],"required":true,"transliteration":true},{"id":"addressLine2","description":"addressLine2","labelName":{"eng":"Address Line2","fra":"Adresse 2"},"controlType":"textbox","inputRequired":true,"fieldType":"default","type":"simpleType","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[]}],"required":false,"transliteration":true},{"id":"addressLine3","description":"addressLine3","labelName":{"eng":"Address Line3","fra":"Adresse 3"},"controlType":"textbox","inputRequired":true,"fieldType":"default","type":"simpleType","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[]}],"required":false,"transliteration":true},{"id":"region","description":"region","labelName":{"eng":"Region","fra":"Région"},"controlType":"dropdown","inputRequired":true,"fieldType":"default","type":"simpleType","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[]}],"parentLocCode":"MOR","locationHierarchyLevel":1,"required":true},{"id":"province","description":"province","labelName":{"eng":"Province","fra":"Province"},"controlType":"dropdown","inputRequired":true,"fieldType":"default","type":"simpleType","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[]}],"locationHierarchyLevel":2,"required":true},{"id":"city","description":"city","labelName":{"eng":"City","fra":"Ville"},"controlType":"dropdown","inputRequired":true,"fieldType":"default","type":"simpleType","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[]}],"locationHierarchyLevel":3,"required":true},{"id":"zone","description":"zone","labelName":{"eng":"Zone","fra":"Zone"},"controlType":"dropdown","inputRequired":true,"fieldType":"default","type":"simpleType","validators":[],"locationHierarchyLevel":4,"required":true},{"id":"postalCode","description":"postalCode","labelName":{"eng":"Postal Code","fra":"code postal"},"controlType":"dropdown","inputRequired":true,"fieldType":"default","type":"string","validators":[{"type":"regex","validator":"^[(?i)A-Z0-9]{5}$|^NA$","arguments":[]}],"locationHierarchyLevel":5,"required":true},{"id":"phone","description":"phone","labelName":{"eng":"Phone","fra":"Téléphone"},"controlType":"textbox","inputRequired":true,"fieldType":"default","type":"string","validators":[{"type":"regex","validator":"^([6-9]{1})([0-9]{9})$","arguments":[]}],"required":true},{"id":"email","description":"email","labelName":{"eng":"Email","fra":"Email"},"controlType":"textbox","inputRequired":true,"fieldType":"default","type":"string","validators":[{"type":"regex","validator":"^[\\w-\\+]+(\\.[\\w]+)*@[\\w-]+(\\.[\\w]+)*(\\.[a-zA-Z]{2,})$","arguments":[]}],"required":true},{"id":"proofOfAddress","description":"proofOfAddress","labelName":{"fra":"Address Proof","eng":"Address Proof"},"controlType":"fileupload","inputRequired":true,"validators":[],"subType":"POA","required":false},{"id":"proofOfIdentity","description":"proofOfIdentity","labelName":{"fra":"Identity Proof","eng":"Identity Proof"},"controlType":"fileupload","inputRequired":true,"validators":[],"subType":"POI","required":true},{"id":"proofOfRelationship","description":"proofOfRelationship","labelName":{"fra":"Relationship Proof","eng":"Relationship Proof"},"controlType":"fileupload","inputRequired":true,"validators":[],"subType":"POR","required":true},{"id":"proofOfDateOfBirth","description":"proofOfDateOfBirth","labelName":{"fra":"DOB Proof","eng":"DOB Proof"},"controlType":"fileupload","inputRequired":true,"validators":[],"subType":"POB","required":true},{"id":"proofOfException","description":"proofOfException","labelName":{"fra":"Exception Proof","eng":"Exception Proof"},"controlType":"fileupload","inputRequired":true,"validators":[],"subType":"POE","required":true},{"id":"proofOfException-1","description":"proofOfException","labelName":{"fra":"Exception Proof","eng":"Exception Proof"},"controlType":"fileupload","inputRequired":true,"validators":[],"subType":"POE","required":true}],"locationHierarchy":["region","province","city","zone","postalCode"]}}</t>
+    <t>[{"id":"IDSchemaVersion","inputRequired":false,"type":"number","minimum":0,"maximum":0,"description":"ID Schema Version","label":{"eng":"IDSchemaVersion"},"controlType":null,"fieldType":"default","format":"none","validators":[],"fieldCategory":"none","alignmentGroup":null,"visible":null,"contactType":null,"group":null,"groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"IdSchemaVersion"},{"id":"UIN","inputRequired":false,"type":"string","minimum":0,"maximum":0,"description":"UIN","label":{"eng":"UIN"},"controlType":"textbox","fieldType":"default","format":"none","validators":[],"fieldCategory":"none","alignmentGroup":null,"visible":null,"contactType":null,"group":null,"groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"UIN"},{"id":"fullName","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"Full Name","label":{"ara":"الاسم الكامل","fra":"Nom complet","eng":"Full Name"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"FullName","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"name"},{"id":"dateOfBirth","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"dateOfBirth","label":{"ara":"الاسم الكامل","fra":"DOB","eng":"DOB"},"controlType":"ageDate","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])/([0][1-9]|1[0-2])/([0][1-9]|[1-2][0-9]|3[01])$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"DateOfBirth","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.isNew || (identity.isUpdate &amp;&amp; (identity.updatableFieldGroups contains 'IntroducerDetails' || identity.updatableFieldGroups contains 'DateOfBirth'))"}],"subType":"dateOfBirth"},{"id":"gender","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"gender","label":{"ara":"جنس","fra":"Le genre","eng":"Gender"},"controlType":"dropdown","fieldType":"dynamic","format":"","validators":[],"fieldCategory":"pvt","alignmentGroup":"group1","visible":null,"contactType":null,"group":"Gender","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"gender"},{"id":"addressLine1","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine1","label":{"ara":"الاسم الكامل","fra":"line1","eng":"line1"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"addressLine1"},{"id":"addressLine2","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine2","label":{"ara":"الاسم الكامل","fra":"line2","eng":"line2"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"addressLine2"},{"id":"addressLine3","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine3","label":{"ara":"الاسم الكامل","fra":"line3","eng":"line3"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"addressLine3"},{"id":"residenceStatus","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"residenceStatus","label":{"ara":"الاسم الكامل","fra":"Reside Status","eng":"Residence Status"},"controlType":"dropdown","fieldType":"dynamic","format":"none","validators":[],"fieldCategory":"kyc","alignmentGroup":"group1","visible":null,"contactType":null,"group":"ResidenceStatus","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"residenceStatus"},{"id":"referenceIdentityNumber","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"referenceIdentityNumber","label":{"ara":"الاسم الكامل","fra":"Reference Identity Number","eng":"Reference Identity Number"},"controlType":"textbox","fieldType":"default","format":"kyc","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"ReferenceIdentityNumber","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"none"},{"id":"region","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"region","label":{"ara":"الاسم الكامل","fra":"Region","eng":"Region"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Region"},{"id":"province","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"province","label":{"ara":"الاسم الكامل","fra":"Province","eng":"Province"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Province"},{"id":"city","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"city","label":{"ara":"الاسم الكامل","fra":"City","eng":"City"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"City"},{"id":"zone","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"zone","label":{"ara":"الاسم الكامل","fra":"Zone","eng":"Zone"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":null,"group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Zone"},{"id":"postalCode","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"postalCode","label":{"ara":"الاسم الكامل","fra":"Postal","eng":"Postal"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[(?i)A-Z0-9]{5}$|^NA$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Postal Code"},{"id":"phone","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"phone","label":{"ara":"الاسم الكامل","fra":"Phone","eng":"Phone"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[+]*([0-9]{1})([0-9]{9})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"contact","visible":null,"contactType":"email","group":"Phone","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Phone"},{"id":"email","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"email","label":{"ara":"الاسم الكامل","fra":"Email","eng":"Email"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[A-Za-z0-9_\\-]+(\\.[A-Za-z0-9_]+)*@[A-Za-z0-9_-]+(\\.[A-Za-z0-9_]+)*(\\.[a-zA-Z]{2,})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"contact","visible":null,"contactType":"email","group":"Email","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Email"},{"id": "introducerName","inputRequired": true,"type": "simpleType","minimum": 0,"maximum": 0,"description": "introducerName","label": {"ara": "اسم المُعرّف","fra":"nom del'introducteur","eng": "Introducer Name"},"controlType": "textbox","fieldType": "default","format": "none","validators": [],"fieldCategory": "evidence","alignmentGroup": "introducer","visible": null,"contactType": null,"group": "IntroducerDetails","groupLabel": null,"changeAction": null,"transliterate": false,"templateName": null,"fieldLayout": null,"locationHierarchy": null,"required": false,"bioAttributes": null,"requiredOn": [{"engine": "MVEL","expr": "( identity.isNew &amp;&amp; identity.isChild ) || ( identity.isUpdate &amp;&amp; identity.isChild ) || ( !(identity.get('introducerRID') == nil || identity.get('introducerRID') == empty) || !(identity.get('introducerUIN') == nil || identity.get('introducerUIN') == empty))"}],"subType": "introducerName"},{"id": "introducerRID","inputRequired": true,"type": "string","minimum": 0,"maximum": 0,"description": "introducerRID","label": {"ara": "مقدم RID","fra": "Introducteur RID","eng": "Introducer RID"},"controlType": "textbox","fieldType": "default","format": "none","validators": [{"type": "regex","validator": "^([0-9]{10,30})$","arguments": [],"langCode": null}],"fieldCategory": "evidence","alignmentGroup": "introducer","visible": null,"contactType": null,"group": "IntroducerDetails","groupLabel": null,"changeAction": null,"transliterate": false,"templateName": null,"fieldLayout": null,"locationHierarchy": null,"required": false,"bioAttributes": null,"requiredOn": [{"engine": "MVEL","expr": "( !(identity.get('introducerName') == nil || identity.get('introducerName') == empty) &amp;&amp; (identity.get('introducerUIN') == nil || identity.get('introducerUIN') == empty))"}],"subType": "RID"},{"id": "introducerUIN","inputRequired": true,"type": "string","minimum": 0,"maximum": 0,"description": "introducerUIN","label": {"ara": "مقدم في","fra": "Introducteur UIN","eng": "Introducer UIN"},"controlType": "textbox","fieldType": "default","format": "none","validators": [{"type": "regex","validator": "^([0-9]{10,30})$","arguments": [],"langCode": null}],"fieldCategory": "evidence","alignmentGroup": "introducer","visible": null,"contactType": null,"group": "IntroducerDetails","groupLabel": null,"changeAction": null,"transliterate": false,"templateName": null,"fieldLayout": null,"locationHierarchy": null,"required": false,"bioAttributes": null,"requiredOn": [{"engine": "MVEL","expr": "( !(identity.get('introducerName') == nil || identity.get('introducerName') == empty) &amp;&amp; (identity.get('introducerRID') == nil || identity.get('introducerRID') == empty))"}],"subType": "UIN"},{"id":"proofOfAddress","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfAddress","label":{"ara":"إثبات العنوان","fra":"Address Proof","eng":"Address Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.isNew || ( identity.isUpdate &amp;&amp; (identity.updatableFields contains 'addressLine1' || identity.updatableFields contains 'addressLine2' || identity.updatableFields contains 'addressLine3'))"}],"subType":"POA"},{"id":"proofOfIdentity","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfIdentity","label":{"ara":"إثبات الهوية","fra":"Identity Proof","eng":"Identity Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.isNew || ( identity.isUpdate &amp;&amp; identity.updatableFields contains 'fullName')"}],"subType":"POI"},{"id":"proofOfRelationship","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfRelationship","label":{"ara":"إثبات العلاقة","fra":"Relationship Proof","eng":"Relationship Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"( identity.isNew &amp;&amp; identity.isChild ) || ( identity.isUpdate &amp;&amp; (identity.updatableFieldGroups contains 'IntroducerDetails' || identity.isChild))"}],"subType":"POR"},{"id":"proofOfDateOfBirth","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfDateOfBirth","label":{"ara":"دليل DOB","fra":"DOB Proof","eng":"DOB Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.isUpdate &amp;&amp; identity.updatableFields contains 'dateOfBirth'"}],"subType":"POB"},{"id":"proofOfException","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfException","label":{"ara":"إثبات الاستثناء","fra":"Exception Proof","eng":"Exception Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"POE"},{"id":"proofOfException-1","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfException","label":{"ara":"إثبات الاستثناء2","fra":"Exception Proof","eng":"Exception Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"POE"},{"id":"individualBiometrics","inputRequired":true,"type":"biometricsType","minimum":0,"maximum":0,"description":"","label":{"ara":"القياسات الحيوية الفردية","fra":"Applicant Biometrics","eng":"Applicant Biometrics"},"controlType":"biometrics","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Biometrics","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"requiredOn":[{"engine":"MVEL","expr":"(identity.isNew || identity.isLost || ( identity.isUpdate &amp;&amp; identity.updatableFieldGroups contains 'Biometrics'))"}],"subType":"applicant"},{"id":"individualAuthBiometrics","inputRequired":true,"type":"biometricsType","minimum":0,"maximum":0,"description":"Used to hold biometrics only for authentication","label":{"ara":"القياسات الحيوية الفردية","fra":"Authentication Biometrics","eng":"Authentication Biometrics"},"controlType":"biometrics","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":null,"groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":false,"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"requiredOn":[{"engine":"MVEL","expr":"!identity.isChild &amp;&amp; identity.isUpdate &amp;&amp; !(identity.updatableFieldGroups contains 'Biometrics' || identity.updatableFieldGroups contains 'IntroducerDetails')"}],"subType":"applicant-auth"},{"id": "introducerBiometrics","inputRequired": true,"type": "biometricsType","minimum": 0,"maximum": 0,"description": "","label": {"ara": "مقدم القياسات الحيوية","fra": "Introducteur Biométrie","eng": "Introducer Biometrics"},"controlType": "biometrics","fieldType": "default","format": "none","validators": [],"fieldCategory": "pvt","alignmentGroup": null,"visible": null,"contactType": null,"group": "Biometrics","groupLabel": null,"changeAction": null,"transliterate": false,"templateName": null,"fieldLayout": null,"locationHierarchy": null,"required": false,"bioAttributes": ["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"requiredOn": [{"engine": "MVEL","expr": "(identity.isChild &amp;&amp; identity.isNew) || (identity.isUpdate &amp;&amp; identity.updatableFieldGroups contains 'IntroducerDetails') || !(identity.get('introducerName') == nil || identity.get('introducerName') == empty)"}],"subType": "introducer"},{"id":"consentText","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"Consent","label":{},"controlType":"html","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"consentText","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":"Registration Consent","fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"consentText"},{"id":"consent","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"consent accepted","label":{"ara":"الاسم الكامل الكامل الكامل","fra":"J'ai lu et j'accepte les termes et conditions pour partager mes PII","eng":"I have read and accept terms and conditions to share my PII"},"controlType":"checkbox","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"consent","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"consent"}]</t>
+  </si>
+  <si>
+    <t>[{"order":1,"name":"ConsentDetails","label":{"ara":"موافقة","fra":"Consentement","eng":"Consent"},"caption":{"ara":"موافقة","fra":"Consentement","eng":"Consent"},"fields":["consentText","consent"],"layoutTemplate":null,"preRegFetchRequired":false,"active":false},{"order":2,"name":"DemographicDetails","label":{"ara":"التفاصيل الديموغرافية","fra":"Détails démographiques","eng":"Demographic Details"},"caption":{"ara":"التفاصيل الديموغرافية","fra":"Détails démographiques","eng":"Demographic Details"},"fields":["fullName","dateOfBirth","gender","residenceStatus","addressLine1","addressLine2","addressLine3","referenceIdentityNumber","region","province","city","zone","postalCode","phone","email","introducerName","introducerRID","introducerUIN"],"layoutTemplate":null,"preRegFetchRequired":true,"active":false},{"order":3,"name":"DocumentsDetails","label":{"ara":"تحميل الوثيقة","fra":"Des documents","eng":"Document Upload"},"caption":{"ara":"وثائق","fra":"Des documents","eng":"Documents"},"fields":["proofOfAddress","proofOfIdentity","proofOfRelationship","proofOfDateOfBirth","proofOfException","proofOfException-1"],"layoutTemplate":null,"preRegFetchRequired":false,"active":false},{"order":4,"name":"BiometricDetails","label":{"ara":"التفاصيل البيومترية","fra":"Détails biométriques","eng":"Biometric Details"},"caption":{"ara":"التفاصيل البيومترية","fra":"Détails biométriques","eng":"Biometric Details"},"fields":["individualBiometrics","individualAuthBiometrics","introducerBiometrics"],"layoutTemplate":null,"preRegFetchRequired":false,"active":false}]</t>
+  </si>
+  <si>
+    <t>cd005fa3-49bd-4de4-8634-81372b707fd1</t>
+  </si>
+  <si>
+    <t>Pre-registration UI Specification for Data capture</t>
+  </si>
+  <si>
+    <t>{"identity":{"identity":[{"id":"IDSchemaVersion","description":"ID Schema Version","type":"number","controlType":null,"fieldType":"default","inputRequired":false,"validators":[],"required":true},{"id":"fullName","description":"Enter Full Name","labelName":{"eng":"Full Name","ara":"الاسم الكامل","fra":"Nom complet"},"controlType":"textbox","inputRequired":true,"fieldType":"default","type":"simpleType","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[]}],"required":true,"transliteration":true},{"id":"dateOfBirth","description":"Enter DOB","labelName":{"eng":"Date Of Birth","ara":"تاريخ الولادة","fra":"Date de naissance"},"controlType":"ageDate","inputRequired":true,"fieldType":"default","type":"string","validators":[],"required":true},{"id":"gender","description":"Enter Gender","labelName":{"eng":"Gender","ara":"جنس","fra":"Le genre"},"controlType":"dropdown","inputRequired":true,"fieldType":"dynamic","subType":"gender","type":"simpleType","validators":[],"required":true},{"id":"residenceStatus","description":"Residence status","labelName":{"eng":"Residence Status","ara":"حالة الإقامة","fra":"Statut de résidence"},"controlType":"dropdown","inputRequired":true,"fieldType":"dynamic","subType":"residenceStatus","type":"simpleType","validators":[],"required":true},{"id":"addressLine1","description":"addressLine1","labelName":{"eng":"Address Line1","ara":"العنوان السطر 1","fra":"Adresse 1"},"controlType":"textbox","inputRequired":true,"fieldType":"default","type":"simpleType","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[]}],"required":true,"transliteration":true},{"id":"addressLine2","description":"addressLine2","labelName":{"eng":"Address Line2","ara":"العنوان السطر 2","fra":"Adresse 2"},"controlType":"textbox","inputRequired":true,"fieldType":"default","type":"simpleType","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[]}],"required":false,"transliteration":true},{"id":"addressLine3","description":"addressLine3","labelName":{"eng":"Address Line3","ara":"العنوان السطر 3","fra":"Adresse 3"},"controlType":"textbox","inputRequired":true,"fieldType":"default","type":"simpleType","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[]}],"required":false,"transliteration":true},{"id":"region","description":"region","labelName":{"eng":"Region","ara":"منطقة","fra":"Région"},"controlType":"dropdown","inputRequired":true,"fieldType":"default","type":"simpleType","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[]}],"parentLocCode":"MOR","locationHierarchyLevel":1,"required":true},{"id":"province","description":"province","labelName":{"eng":"Province","ara":"المحافظة","fra":"Province"},"controlType":"dropdown","inputRequired":true,"fieldType":"default","type":"simpleType","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[]}],"locationHierarchyLevel":2,"required":true},{"id":"city","description":"city","labelName":{"eng":"City","ara":"مدينة","fra":"Ville"},"controlType":"dropdown","inputRequired":true,"fieldType":"default","type":"simpleType","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[]}],"locationHierarchyLevel":3,"required":true},{"id":"zone","description":"zone","labelName":{"eng":"Zone","ara":"منطقة","fra":"Zone"},"controlType":"dropdown","inputRequired":true,"fieldType":"default","type":"simpleType","validators":[],"locationHierarchyLevel":4,"required":true},{"id":"postalCode","description":"postalCode","labelName":{"eng":"Postal Code","ara":"الكود البريدى","fra":"code postal"},"controlType":"dropdown","inputRequired":true,"fieldType":"default","type":"string","validators":[{"type":"regex","validator":"^[(?i)A-Z0-9]{5}$|^NA$","arguments":[]}],"locationHierarchyLevel":5,"required":true},{"id":"phone","description":"phone","labelName":{"eng":"Phone","ara":"هاتف","fra":"Téléphone"},"controlType":"textbox","inputRequired":true,"fieldType":"default","type":"string","validators":[{"type":"regex","validator":"^([6-9]{1})([0-9]{9})$","arguments":[]}],"required":true},{"id":"email","description":"email","labelName":{"eng":"Email","ara":"البريد الإلكتروني","fra":"Email"},"controlType":"textbox","inputRequired":true,"fieldType":"default","type":"string","validators":[{"type":"regex","validator":"^[\\w-\\+]+(\\.[\\w]+)*@[\\w-]+(\\.[\\w]+)*(\\.[a-zA-Z]{2,})$","arguments":[]}],"required":true},{"id":"proofOfAddress","description":"proofOfAddress","labelName":{"ara":"إثبات العنوان","fra":"Address Proof","eng":"Address Proof"},"controlType":"fileupload","inputRequired":true,"validators":[],"subType":"POA","required":false},{"id":"proofOfIdentity","description":"proofOfIdentity","labelName":{"ara":"إثبات الهوية","fra":"Identity Proof","eng":"Identity Proof"},"controlType":"fileupload","inputRequired":true,"validators":[],"subType":"POI","required":true},{"id":"proofOfRelationship","description":"proofOfRelationship","labelName":{"ara":"إثبات العلاقة","fra":"Relationship Proof","eng":"Relationship Proof"},"controlType":"fileupload","inputRequired":true,"validators":[],"subType":"POR","required":true},{"id":"proofOfDateOfBirth","description":"proofOfDateOfBirth","labelName":{"ara":"دليل DOB","fra":"DOB Proof","eng":"DOB Proof"},"controlType":"fileupload","inputRequired":true,"validators":[],"subType":"POB","required":true},{"id":"proofOfException","description":"proofOfException","labelName":{"ara":"إثبات الاستثناء","fra":"Exception Proof","eng":"Exception Proof"},"controlType":"fileupload","inputRequired":true,"validators":[],"subType":"POE","required":true},{"id":"proofOfException-1","description":"proofOfException","labelName":{"ara":"إثبات الاستثناء 2","fra":"Exception Proof","eng":"Exception Proof"},"controlType":"fileupload","inputRequired":true,"validators":[],"subType":"POE","required":true}],"locationHierarchy":["region","province","city","zone","postalCode"]}}</t>
+  </si>
+  <si>
+    <t>service-account-mosip-reg-client</t>
+  </si>
+  <si>
+    <t>c1ef9f1c-b1b6-4c78-871f-000ed543c191</t>
+  </si>
+  <si>
+    <t>New Registration process</t>
+  </si>
+  <si>
+    <t>{"id":"NEW","order":1,"flow":"NEW","isSubProcess":false,"label":{"eng":"New Registration","ara":"تسجيل جديد","fra":"Nouvelle inscription"},"screens":[{"order":1,"name":"consentdet","label":{"ara":"موافقة","fra":"Consentement","eng":"Consent"},"caption":{"ara":"موافقة","fra":"Consentement","eng":"Consent"},"fields":[{"id":"IDSchemaVersion","inputRequired":false,"type":"number","minimum":0,"maximum":0,"description":"ID Schema Version","label":{"eng":"IDSchemaVersion"},"controlType":null,"fieldType":"default","format":"none","validators":[],"fieldCategory":"none","alignmentGroup":null,"visible":null,"contactType":null,"group":null,"groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"IdSchemaVersion"},{"id":"consentText","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"Consent","label":{},"controlType":"html","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"consentText","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":"Registration Consent","fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"consentText"},{"id":"consent","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"consent accepted","label":{"ara":"الاسم الكامل الكامل الكامل","fra":"J'ai lu et j'accepte les termes et conditions pour partager mes PII","eng":"I have read and accept terms and conditions to share my PII"},"controlType":"checkbox","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"consent","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"consent"},{"id":"preferredLang","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"user preferred Language","label":{"ara":"لغة الإخطار","fra":"Langue de notification","eng":"Notification Langauge"},"controlType":"button","fieldType":"dynamic","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":"group1","visible":null,"contactType":null,"group":"PreferredLanguage","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"preferredLang"}],"layoutTemplate":null,"preRegFetchRequired":false,"active":false},{"order":2,"name":"DemographicDetails","label":{"ara":"التفاصيل الديموغرافية","fra":"Détails démographiques","eng":"Demographic Details"},"caption":{"ara":"التفاصيل الديموغرافية","fra":"Détails démographiques","eng":"Demographic Details"},"fields":[{"id":"fullName","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"Full Name","label":{"ara":"الاسم الكامل","fra":"Nom complet","eng":"Full Name"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"FullName","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"name"},{"id":"dateOfBirth","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"dateOfBirth","label":{"ara":"الاسم الكامل","fra":"DOB","eng":"DOB"},"controlType":"ageDate","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])/([0][1-9]|1[0-2])/([0][1-9]|[1-2][0-9]|3[01])$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"DateOfBirth","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"dateOfBirth"},{"id":"gender","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"gender","label":{"ara":"جنس","fra":"Le genre","eng":"Gender"},"controlType":"button","fieldType":"dynamic","format":"","validators":[],"fieldCategory":"pvt","alignmentGroup":"group1","visible":null,"contactType":null,"group":"Gender","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"gender"},{"id":"addressLine1","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine1","label":{"ara":"الاسم الكامل","fra":"line1","eng":"line1"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"addressLine1"},{"id":"addressLine2","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine2","label":{"ara":"الاسم الكامل","fra":"line2","eng":"line2"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"addressLine2"},{"id":"addressLine3","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine3","label":{"ara":"الاسم الكامل","fra":"line3","eng":"line3"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"addressLine3"},{"id":"residenceStatus","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"residenceStatus","label":{"ara":"الاسم الكامل","fra":"Reside Status","eng":"Residence Status"},"controlType":"button","fieldType":"dynamic","format":"none","validators":[],"fieldCategory":"kyc","alignmentGroup":"group1","visible":null,"contactType":null,"group":"ResidenceStatus","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"residenceStatus"},{"id":"referenceIdentityNumber","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"referenceIdentityNumber","label":{"ara":"الاسم الكامل","fra":"Reference Identity Number","eng":"Reference Identity Number"},"controlType":"textbox","fieldType":"default","format":"kyc","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"ReferenceIdentityNumber","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"none"},{"id":"region","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"region","label":{"ara":"الاسم الكامل","fra":"Region","eng":"Region"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Region"},{"id":"province","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"province","label":{"ara":"الاسم الكامل","fra":"Province","eng":"Province"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Province"},{"id":"city","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"city","label":{"ara":"الاسم الكامل","fra":"City","eng":"City"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"City"},{"id":"zone","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"zone","label":{"ara":"الاسم الكامل","fra":"Zone","eng":"Zone"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":null,"group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Zone"},{"id":"postalCode","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"postalCode","label":{"ara":"الاسم الكامل","fra":"Postal","eng":"Postal"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[(?i)A-Z0-9]{5}$|^NA$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Postal Code"},{"id":"phone","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"phone","label":{"ara":"الاسم الكامل","fra":"Phone","eng":"Phone"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[+]*([0-9]{1})([0-9]{9})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"contact","visible":null,"contactType":"email","group":"Phone","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Phone"},{"id":"email","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"email","label":{"ara":"الاسم الكامل","fra":"Email","eng":"Email"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[A-Za-z0-9_\\-]+(\\.[A-Za-z0-9_]+)*@[A-Za-z0-9_-]+(\\.[A-Za-z0-9_]+)*(\\.[a-zA-Z]{2,})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"contact","visible":null,"contactType":"email","group":"Email","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Email"},{"id":"introducerName","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"introducerName","label":{"ara":"اسم المُعرّف","fra":"nom del'introducteur","eng":"Introducer Name"},"controlType":"textbox","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT'"},"contactType":null,"group":"IntroducerDetails","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT'"}],"subType":"introducerName"},{"id":"introducerRID","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"introducerRID","label":{"ara":"مقدم RID","fra":"Introducteur RID","eng":"Introducer RID"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT' &amp;&amp; (identity.get('introducerUIN') == nil || identity.get('introducerUIN') == empty)"},"contactType":null,"group":"IntroducerDetails","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT' &amp;&amp; (identity.get('introducerUIN') == nil || identity.get('introducerUIN') == empty)"}],"subType":"RID"},{"id":"introducerUIN","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"introducerUIN","label":{"ara":"مقدم في","fra":"Introducteur UIN","eng":"Introducer UIN"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT' &amp;&amp; (identity.get('introducerRID') == nil || identity.get('introducerRID') == empty)"},"contactType":null,"group":"IntroducerDetails","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT' &amp;&amp; (identity.get('introducerRID') == nil || identity.get('introducerRID') == empty)"}],"subType":"UIN"}],"layoutTemplate":null,"preRegFetchRequired":true,"active":false},{"order":3,"name":"Documents","label":{"ara":"تحميل الوثيقة","fra":"Des documents","eng":"Document Upload"},"caption":{"ara":"وثائق","fra":"Des documents","eng":"Documents"},"fields":[{"id":"proofOfAddress","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfAddress","label":{"ara":"إثبات العنوان","fra":"Address Proof","eng":"Address Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"POA"},{"id":"proofOfIdentity","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfIdentity","label":{"ara":"إثبات الهوية","fra":"Identity Proof","eng":"Identity Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"POI"},{"id":"proofOfRelationship","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfRelationship","label":{"ara":"إثبات العلاقة","fra":"Relationship Proof","eng":"Relationship Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT'"}],"subType":"POR"},{"id":"proofOfDateOfBirth","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfDateOfBirth","label":{"ara":"دليل DOB","fra":"DOB Proof","eng":"DOB Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"POB"},{"id":"proofOfException","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfException","label":{"ara":"إثبات الاستثناء","fra":"Exception Proof","eng":"Exception Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"POE"}],"layoutTemplate":null,"preRegFetchRequired":false,"active":false},{"order":4,"name":"BiometricDetails","label":{"ara":"التفاصيل البيومترية","fra":"Détails biométriques","eng":"Biometric Details"},"caption":{"ara":"التفاصيل البيومترية","fra":"Détails biométriques","eng":"Biometric Details"},"fields":[{"id":"individualBiometrics","inputRequired":true,"type":"biometricsType","minimum":0,"maximum":0,"description":"","label":{"ara":"القياسات الحيوية الفردية","fra":"Applicant Biometrics","eng":"Applicant Biometrics"},"controlType":"biometrics","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Biometrics","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":[{"ageGroup":"INFANT","process":"ALL","validationExpr":"face","bioAttributes":["face"]}],"required":true,"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"requiredOn":[],"subType":"applicant"},{"id":"introducerBiometrics","inputRequired":true,"type":"biometricsType","minimum":0,"maximum":0,"description":"","label":{"ara":"مقدم القياسات الحيوية","fra":"Introducteur Biométrie","eng":"Introducer Biometrics"},"controlType":"biometrics","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Biometrics","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":[{"ageGroup":"INFANT","process":"ALL","validationExpr":"leftEye || rightEye || rightIndex || rightLittle || rightRing || rightMiddle || leftIndex || leftLittle || leftRing || leftMiddle || leftThumb || rightThumb || face","bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"]}],"required":false,"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"requiredOn":[{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT'"}],"subType":"introducer"}],"layoutTemplate":null,"preRegFetchRequired":false,"active":false}],"caption":{"eng":"New Registration","ara":"تسجيل جديد","fra":"Nouvelle inscription"},"icon":"NewReg.png","isActive":true,"autoSelectedGroups":null}</t>
+  </si>
+  <si>
+    <t>703796d8-085f-4778-80be-df298c1b8367</t>
+  </si>
+  <si>
+    <t>Update Registration process</t>
+  </si>
+  <si>
+    <t>{"id":"UPDATE","order":2,"flow":"UPDATE","isSubProcess":false,"label":{"eng":"Update UIN","ara":"تحديث UIN","fra":"Mettre à jour l'UIN"},"screens":[{"order":1,"name":"consentdet","label":{"ara":"موافقة","fra":"Consentement","eng":"Consent"},"caption":{"ara":"موافقة","fra":"Consentement","eng":"Consent"},"fields":[{"id":"consentText","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"Consent","label":{},"controlType":"html","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"Consent","groupLabel":{"ara":"موافقة","fra":"Consentement","eng":"Consent"},"changeAction":null,"transliterate":false,"templateName":"Registration Consent","fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"consentText"},{"id":"consent","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"consent accepted","label":{"ara":"الاسم الكامل الكامل الكامل","fra":"J'ai lu et j'accepte les termes et conditions pour partager mes PII","eng":"I have read and accept terms and conditions to share my PII"},"controlType":"checkbox","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"Consent","groupLabel":{"ara":"موافقة","fra":"Consentement","eng":"Consent"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"consent"},{"id":"preferredLang","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"user preferred Language","label":{"ara":"لغة الإخطار","fra":"Langue de notification","eng":"Notification Langauge"},"controlType":"button","fieldType":"dynamic","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":"group1","visible":null,"contactType":null,"group":"PreferredLanguage","groupLabel":{"ara":"لغة الإخطار","fra":"Langue de notification","eng":"Notification Langauge"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"preferredLang"}],"layoutTemplate":null,"preRegFetchRequired":false,"active":false},{"order":2,"name":"DemographicDetails","label":{"ara":"التفاصيل الديموغرافية","fra":"Détails démographiques","eng":"Demographic Details"},"caption":{"ara":"التفاصيل الديموغرافية","fra":"Détails démographiques","eng":"Demographic Details"},"fields":[{"id":"fullName","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"Full Name","label":{"ara":"الاسم الكامل","fra":"Nom complet","eng":"Full Name"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"FullName","groupLabel":{"ara":"الاسم الكامل","fra":"Nom complet","eng":"Full Name"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"name"},{"id":"dateOfBirth","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"dateOfBirth","label":{"ara":"الاسم الكامل","fra":"DOB","eng":"DOB"},"controlType":"ageDate","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])/([0][1-9]|1[0-2])/([0][1-9]|[1-2][0-9]|3[01])$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"DateOfBirth","groupLabel":{"ara":"تاريخ الولادة","fra":"Date de naissance","eng":"Date Of Birth"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"dateOfBirth"},{"id":"gender","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"gender","label":{"ara":"جنس","fra":"Le genre","eng":"Gender"},"controlType":"button","fieldType":"dynamic","format":"","validators":[],"fieldCategory":"pvt","alignmentGroup":"group1","visible":null,"contactType":null,"group":"Gender","groupLabel":{"ara":"جنس","fra":"Le genre","eng":"Gender"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"gender"},{"id":"addressLine1","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine1","label":{"ara":"الاسم الكامل","fra":"line1","eng":"line1"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":{"ara":"تبوك","fra":"Adresse","eng":"Address"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"addressLine1"},{"id":"addressLine2","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine2","label":{"ara":"الاسم الكامل","fra":"line2","eng":"line2"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":{"ara":"تبوك","fra":"Adresse","eng":"Address"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"addressLine2"},{"id":"addressLine3","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine3","label":{"ara":"الاسم الكامل","fra":"line3","eng":"line3"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":{"ara":"تبوك","fra":"Adresse","eng":"Address"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"addressLine3"},{"id":"residenceStatus","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"residenceStatus","label":{"ara":"الاسم الكامل","fra":"Reside Status","eng":"Residence Status"},"controlType":"button","fieldType":"dynamic","format":"none","validators":[],"fieldCategory":"kyc","alignmentGroup":"group1","visible":null,"contactType":null,"group":"ResidenceStatus","groupLabel":{"ara":"الاسم الكامل","fra":"Reside Status","eng":"Residence Status"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"residenceStatus"},{"id":"referenceIdentityNumber","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"referenceIdentityNumber","label":{"ara":"الاسم الكامل","fra":"Reference Identity Number","eng":"Reference Identity Number"},"controlType":"textbox","fieldType":"default","format":"kyc","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"ReferenceIdentityNumber","groupLabel":{"ara":"الاسم الكامل","fra":"Reference Identity Number","eng":"Reference Identity Number"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"none"},{"id":"region","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"region","label":{"ara":"الاسم الكامل","fra":"Region","eng":"Region"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":{"ara":"موقع","fra":"Lieu","eng":"Location"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Region"},{"id":"province","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"province","label":{"ara":"الاسم الكامل","fra":"Province","eng":"Province"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":{"ara":"موقع","fra":"Lieu","eng":"Location"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Province"},{"id":"city","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"city","label":{"ara":"الاسم الكامل","fra":"City","eng":"City"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":{"ara":"موقع","fra":"Lieu","eng":"Location"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"City"},{"id":"zone","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"zone","label":{"ara":"الاسم الكامل","fra":"Zone","eng":"Zone"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":null,"group":"Location","groupLabel":{"ara":"موقع","fra":"Lieu","eng":"Location"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Zone"},{"id":"postalCode","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"postalCode","label":{"ara":"الاسم الكامل","fra":"Postal","eng":"Postal"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[(?i)A-Z0-9]{5}$|^NA$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":{"ara":"موقع","fra":"Lieu","eng":"Location"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Postal Code"},{"id":"phone","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"phone","label":{"ara":"الاسم الكامل","fra":"Phone","eng":"Phone"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[+]*([0-9]{1})([0-9]{9})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"contact","visible":null,"contactType":"email","group":"Phone","groupLabel":{"ara":"الاسم الكامل","fra":"Phone","eng":"Phone"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Phone"},{"id":"email","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"email","label":{"ara":"الاسم الكامل","fra":"Email","eng":"Email"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[A-Za-z0-9_\\-]+(\\.[A-Za-z0-9_]+)*@[A-Za-z0-9_-]+(\\.[A-Za-z0-9_]+)*(\\.[a-zA-Z]{2,})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"contact","visible":null,"contactType":"email","group":"Email","groupLabel":{"ara":"الاسم الكامل","fra":"Email","eng":"Email"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"Email"},{"id":"introducerName","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"introducerName","label":{"ara":"اسم المُعرّف","fra":"nom del'introducteur","eng":"Introducer Name"},"controlType":"textbox","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":null,"contactType":null,"group":"IntroducerDetails","groupLabel":{"ara":"تفاصيل المعرف","eng":"Introducer Details","fra":"Détails de l'introducteur"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"introducerName"},{"id":"introducerRID","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"introducerRID","label":{"ara":"مقدم RID","fra":"Introducteur RID","eng":"Introducer RID"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":{"engine":"MVEL","expr":"identity.get('introducerUIN') == nil || identity.get('introducerUIN') == empty"},"contactType":null,"group":"IntroducerDetails","groupLabel":{"ara":"تفاصيل المعرف","eng":"Introducer Details","fra":"Détails de l'introducteur"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.get('introducerUIN') == nil || identity.get('introducerUIN') == empty"}],"subType":"RID"},{"id":"introducerUIN","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"introducerUIN","label":{"ara":"مقدم في","fra":"Introducteur UIN","eng":"Introducer UIN"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":{"engine":"MVEL","expr":"identity.get('introducerRID') == nil || identity.get('introducerRID') == empty"},"contactType":null,"group":"IntroducerDetails","groupLabel":{"ara":"تفاصيل المعرف","eng":"Introducer Details","fra":"Détails de l'introducteur"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.get('introducerRID') == nil || identity.get('introducerRID') == empty"}],"subType":"UIN"}],"layoutTemplate":null,"preRegFetchRequired":true,"active":false},{"order":3,"name":"Documents","label":{"ara":"تحميل الوثيقة","fra":"Des documents","eng":"Document Upload"},"caption":{"ara":"وثائق","fra":"Des documents","eng":"Documents"},"fields":[{"id":"proofOfAddress","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfAddress","label":{"ara":"إثبات العنوان","fra":"Address Proof","eng":"Address Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":{"ara":"وثائق","fra":"Documents","eng":"Documents"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.updatableFieldGroups contains 'Address' || identity.updatableFieldGroups contains 'Location'"}],"subType":"POA"},{"id":"proofOfIdentity","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfIdentity","label":{"ara":"إثبات الهوية","fra":"Identity Proof","eng":"Identity Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":{"ara":"وثائق","fra":"Documents","eng":"Documents"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.updatableFieldGroups contains 'FullName' || identity.updatableFieldGroups contains 'DateOfBirth'"}],"subType":"POI"},{"id":"proofOfRelationship","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfRelationship","label":{"ara":"إثبات العلاقة","fra":"Relationship Proof","eng":"Relationship Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":{"ara":"وثائق","fra":"Documents","eng":"Documents"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT' || identity.updatableFieldGroups contains 'IntroducerDetails'"}],"subType":"POR"},{"id":"proofOfDateOfBirth","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfDateOfBirth","label":{"ara":"دليل DOB","fra":"DOB Proof","eng":"DOB Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":{"ara":"وثائق","fra":"Documents","eng":"Documents"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.updatableFieldGroups contains 'DateOfBirth'"}],"subType":"POB"},{"id":"proofOfException","inputRequired":true,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfException","label":{"ara":"إثبات الاستثناء","fra":"Exception Proof","eng":"Exception Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":{"ara":"وثائق","fra":"Documents","eng":"Documents"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"POE"}],"layoutTemplate":null,"preRegFetchRequired":false,"active":false},{"order":4,"name":"BiometricDetails","label":{"ara":"التفاصيل البيومترية","fra":"Détails biométriques","eng":"Biometric Details"},"caption":{"ara":"التفاصيل البيومترية","fra":"Détails biométriques","eng":"Biometric Details"},"fields":[{"id":"individualBiometrics","inputRequired":true,"type":"biometricsType","minimum":0,"maximum":0,"description":"","label":{"ara":"القياسات الحيوية الفردية","fra":"Biométrie du demandeur","eng":"Applicant Biometrics"},"controlType":"biometrics","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Biometrics","groupLabel":{"ara":"القياسات الحيوية","fra":"Biométrie","eng":"Biometrics"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":[{"ageGroup":"INFANT","process":"ALL","validationExpr":"face","bioAttributes":["face"]}],"required":true,"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"requiredOn":[{"engine":"MVEL","expr":"identity.updatableFieldGroups contains 'Biometrics'"}],"subType":"applicant"},{"id":"individualAuthBiometrics","inputRequired":true,"type":"biometricsType","minimum":0,"maximum":0,"description":"Used to hold biometrics only for authentication","label":{"ara":"القياسات الحيوية الفردية","fra":"Authentification Biométrie","eng":"Authentication Biometrics"},"controlType":"biometrics","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Biometrics","groupLabel":{"ara":"القياسات الحيوية","fra":"Biométrie","eng":"Biometrics"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":[{"ageGroup":"ALL","process":"ALL","validationExpr":"leftEye || rightEye || rightIndex || rightLittle || rightRing || rightMiddle || leftIndex || leftLittle || leftRing || leftMiddle || leftThumb || rightThumb || face","bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"]}],"required":false,"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"requiredOn":[{"engine":"MVEL","expr":"!(identity.get('ageGroup') == 'INFANT') &amp;&amp; !(identity.updatableFieldGroups contains 'Biometrics')"}],"subType":"applicant-auth"},{"id":"introducerBiometrics","inputRequired":true,"type":"biometricsType","minimum":0,"maximum":0,"description":"","label":{"ara":"مقدم القياسات الحيوية","fra":"Introducteur Biométrie","eng":"Introducer Biometrics"},"controlType":"biometrics","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Biometrics","groupLabel":{"ara":"القياسات الحيوية","fra":"Biométrie","eng":"Biometrics"},"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":[{"ageGroup":"ALL","process":"ALL","validationExpr":"leftEye || rightEye || rightIndex || rightLittle || rightRing || rightMiddle || leftIndex || leftLittle || leftRing || leftMiddle || leftThumb || rightThumb || face","bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"]}],"required":false,"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"requiredOn":[{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT' || identity.updatableFieldGroups contains 'IntroducerDetails'"}],"subType":"introducer"}],"layoutTemplate":null,"preRegFetchRequired":false,"active":false}],"caption":{"eng":"Update UIN","ara":"تحديث UIN","fra":"Mettre à jour l'UIN"},"icon":"UINUpdate.png","isActive":true,"autoSelectedGroups":["Consent","PreferredLanguage","Documents","Biometrics"]}</t>
+  </si>
+  <si>
+    <t>78f07cba-0f5d-4e28-a970-f85d1ac302c9</t>
+  </si>
+  <si>
+    <t>Lost Registration process</t>
+  </si>
+  <si>
+    <t>{"id":"LOST","order":3,"flow":"LOST","isSubProcess":false,"label":{"eng":"Lost UIN","ara":"فقدت UIN","fra":"UIN perdu"},"screens":[{"order":1,"name":"consentdet","label":{"ara":"موافقة","fra":"Consentement","eng":"Consent"},"caption":{"ara":"موافقة","fra":"Consentement","eng":"Consent"},"fields":[{"id":"IDSchemaVersion","inputRequired":false,"type":"number","minimum":0,"maximum":0,"description":"ID Schema Version","label":{"eng":"IDSchemaVersion"},"controlType":null,"fieldType":"default","format":"none","validators":[],"fieldCategory":"none","alignmentGroup":null,"visible":null,"contactType":null,"group":null,"groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"IdSchemaVersion"},{"id":"consentText","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"Consent","label":{},"controlType":"html","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"consentText","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":"Registration Consent","fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"consentText"},{"id":"consent","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"consent accepted","label":{"ara":"الاسم الكامل الكامل الكامل","fra":"J'ai lu et j'accepte les termes et conditions pour partager mes PII","eng":"I have read and accept terms and conditions to share my PII"},"controlType":"checkbox","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"consent","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"consent"},{"id":"preferredLang","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"user preferred Language","label":{"ara":"لغة الإخطار","fra":"Langue de notification","eng":"Notification Langauge"},"controlType":"button","fieldType":"dynamic","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":"group1","visible":null,"contactType":null,"group":"PreferredLanguage","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"preferredLang"}],"layoutTemplate":null,"preRegFetchRequired":false,"active":false},{"order":2,"name":"DemographicDetails","label":{"ara":"التفاصيل الديموغرافية","fra":"Détails démographiques","eng":"Demographic Details"},"caption":{"ara":"التفاصيل الديموغرافية","fra":"Détails démographiques","eng":"Demographic Details"},"fields":[{"id":"fullName","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"Full Name","label":{"ara":"الاسم الكامل","fra":"Nom complet","eng":"Full Name"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"FullName","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"name"},{"id":"dateOfBirth","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"dateOfBirth","label":{"ara":"الاسم الكامل","fra":"DOB","eng":"DOB"},"controlType":"ageDate","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(1869|18[7-9][0-9]|19[0-9][0-9]|20[0-9][0-9])/([0][1-9]|1[0-2])/([0][1-9]|[1-2][0-9]|3[01])$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"DateOfBirth","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"dateOfBirth"},{"id":"gender","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"gender","label":{"ara":"جنس","fra":"Le genre","eng":"Gender"},"controlType":"button","fieldType":"dynamic","format":"","validators":[],"fieldCategory":"pvt","alignmentGroup":"group1","visible":null,"contactType":null,"group":"Gender","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"gender"},{"id":"addressLine1","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine1","label":{"ara":"الاسم الكامل","fra":"line1","eng":"line1"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"addressLine1"},{"id":"addressLine2","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine2","label":{"ara":"الاسم الكامل","fra":"line2","eng":"line2"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"addressLine2"},{"id":"addressLine3","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"addressLine3","label":{"ara":"الاسم الكامل","fra":"line3","eng":"line3"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{3,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"address","visible":null,"contactType":"Postal","group":"Address","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"addressLine3"},{"id":"residenceStatus","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"residenceStatus","label":{"ara":"الاسم الكامل","fra":"Reside Status","eng":"Residence Status"},"controlType":"button","fieldType":"dynamic","format":"none","validators":[],"fieldCategory":"kyc","alignmentGroup":"group1","visible":null,"contactType":null,"group":"ResidenceStatus","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"residenceStatus"},{"id":"referenceIdentityNumber","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"referenceIdentityNumber","label":{"ara":"الاسم الكامل","fra":"Reference Identity Number","eng":"Reference Identity Number"},"controlType":"textbox","fieldType":"default","format":"kyc","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"ReferenceIdentityNumber","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"none"},{"id":"region","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"region","label":{"ara":"الاسم الكامل","fra":"Region","eng":"Region"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"Region"},{"id":"province","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"province","label":{"ara":"الاسم الكامل","fra":"Province","eng":"Province"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"Province"},{"id":"city","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"city","label":{"ara":"الاسم الكامل","fra":"City","eng":"City"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^(?=.{0,50}$).*","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"City"},{"id":"zone","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"zone","label":{"ara":"الاسم الكامل","fra":"Zone","eng":"Zone"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":null,"group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"Zone"},{"id":"postalCode","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"postalCode","label":{"ara":"الاسم الكامل","fra":"Postal","eng":"Postal"},"controlType":"dropdown","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[(?i)A-Z0-9]{5}$|^NA$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"location","visible":null,"contactType":"Postal","group":"Location","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"Postal Code"},{"id":"phone","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"phone","label":{"ara":"الاسم الكامل","fra":"Phone","eng":"Phone"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[+]*([0-9]{1})([0-9]{9})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"contact","visible":null,"contactType":"email","group":"Phone","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"Phone"},{"id":"email","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"email","label":{"ara":"الاسم الكامل","fra":"Email","eng":"Email"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^[A-Za-z0-9_\\-]+(\\.[A-Za-z0-9_]+)*@[A-Za-z0-9_-]+(\\.[A-Za-z0-9_]+)*(\\.[a-zA-Z]{2,})$","arguments":[],"langCode":null}],"fieldCategory":"pvt","alignmentGroup":"contact","visible":null,"contactType":"email","group":"Email","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"Email"},{"id":"introducerName","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"introducerName","label":{"ara":"اسم المُعرّف","fra":"nom del'introducteur","eng":"Introducer Name"},"controlType":"textbox","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT'"},"contactType":null,"group":"IntroducerDetails","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT'"}],"subType":"introducerName"},{"id":"introducerRID","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"introducerRID","label":{"ara":"مقدم RID","fra":"Introducteur RID","eng":"Introducer RID"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT' &amp;&amp; (identity.get('introducerUIN') == nil || identity.get('introducerUIN') == empty)"},"contactType":null,"group":"IntroducerDetails","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT' &amp;&amp; (identity.get('introducerUIN') == nil || identity.get('introducerUIN') == empty)"}],"subType":"RID"},{"id":"introducerUIN","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"introducerUIN","label":{"ara":"مقدم في","fra":"Introducteur UIN","eng":"Introducer UIN"},"controlType":"textbox","fieldType":"default","format":"none","validators":[{"type":"regex","validator":"^([0-9]{10,30})$","arguments":[],"langCode":null}],"fieldCategory":"evidence","alignmentGroup":"introducer","visible":{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT' &amp;&amp; (identity.get('introducerRID') == nil || identity.get('introducerRID') == empty)"},"contactType":null,"group":"IntroducerDetails","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[{"engine":"MVEL","expr":"identity.get('ageGroup') == 'INFANT' &amp;&amp; (identity.get('introducerRID') == nil || identity.get('introducerRID') == empty)"}],"subType":"UIN"}],"layoutTemplate":null,"preRegFetchRequired":true,"active":false},{"order":3,"name":"BiometricDetails","label":{"ara":"التفاصيل البيومترية","fra":"Détails biométriques","eng":"Biometric Details"},"caption":{"ara":"التفاصيل البيومترية","fra":"Détails biométriques","eng":"Biometric Details"},"fields":[{"id":"individualBiometrics","inputRequired":true,"type":"biometricsType","minimum":0,"maximum":0,"description":"","label":{"ara":"القياسات الحيوية الفردية","fra":"Applicant Biometrics","eng":"Applicant Biometrics"},"controlType":"biometrics","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Biometrics","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":[{"ageGroup":"INFANT","process":"ALL","validationExpr":"face","bioAttributes":["face"]}],"required":true,"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"requiredOn":[],"subType":"applicant"},{"id":"proofOfException","inputRequired":false,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfException","label":{"ara":"إثبات الاستثناء","fra":"Exception Proof","eng":"Exception Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"POE"}],"layoutTemplate":null,"preRegFetchRequired":false,"active":false}],"caption":{"eng":"Lost UIN","ara":"فقدت UIN","fra":"UIN perdu"},"icon":"LostUIN.png","isActive":true,"autoSelectedGroups":null}</t>
+  </si>
+  <si>
+    <t>6a080562-86d0-4dba-8bd9-4bdc89243e70</t>
+  </si>
+  <si>
+    <t>Biometric correction Registration process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"id":"BIOMETRIC_CORRECTION","order":4,"flow":"CORRECTION","isSubProcess":false,"label":{"eng":"Biometric correction","ara":"التصحيح البيومتري","fra":"Correction biométrique"},"screens":[{"order":1,"name":"consentdet","label":{"ara":"موافقة","fra":"Consentement","eng":"Consent"},"caption":{"ara":"موافقة","fra":"Consentement","eng":"Consent"},"fields":[{"id":"consentText","inputRequired":true,"type":"simpleType","minimum":0,"maximum":0,"description":"Consent","label":{},"controlType":"html","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"consentText","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":"Registration Consent","fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"consentText"},{"id":"consent","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"consent accepted","label":{"ara":"الاسم الكامل الكامل الكامل","fra":"J'ai lu et j'accepte les termes et conditions pour partager mes PII","eng":"I have read and accept terms and conditions to share my PII"},"controlType":"checkbox","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"consent","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"consent"},{"id":"preferredLang","inputRequired":true,"type":"string","minimum":0,"maximum":0,"description":"user preferred Language","label":{"ara":"لغة الإخطار","fra":"Langue de notification","eng":"Notification Langauge"},"controlType":"button","fieldType":"dynamic","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":"group1","visible":null,"contactType":null,"group":"PreferredLanguage","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":true,"bioAttributes":null,"requiredOn":[],"subType":"preferredLang"}],"layoutTemplate":null,"preRegFetchRequired":false,"additionalInfoRequestIdRequired":false,"active":false},{"order":2,"name":"BiometricDetails","label":{"ara":"التفاصيل البيومترية","fra":"Détails biométriques","eng":"Biometric Details"},"caption":{"ara":"التفاصيل البيومترية","fra":"Détails biométriques","eng":"Biometric Details"},"fields":[{"id":"individualBiometrics","inputRequired":true,"type":"biometricsType","minimum":0,"maximum":0,"description":"","label":{"ara":"القياسات الحيوية الفردية","fra":"Applicant Biometrics","eng":"Applicant Biometrics"},"controlType":"biometrics","fieldType":"default","format":"none","validators":[],"fieldCategory":"pvt","alignmentGroup":null,"visible":null,"contactType":null,"group":"Biometrics","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":[{"ageGroup":"INFANT","process":"ALL","validationExpr":"face","bioAttributes":["face"]}],"required":true,"bioAttributes":["leftEye","rightEye","rightIndex","rightLittle","rightRing","rightMiddle","leftIndex","leftLittle","leftRing","leftMiddle","leftThumb","rightThumb","face"],"requiredOn":[],"subType":"applicant"},{"id":"proofOfException","inputRequired":false,"type":"documentType","minimum":0,"maximum":0,"description":"proofOfException","label":{"ara":"إثبات الاستثناء","fra":"Exception Proof","eng":"Exception Proof"},"controlType":"fileupload","fieldType":"default","format":"none","validators":[],"fieldCategory":"evidence","alignmentGroup":null,"visible":null,"contactType":null,"group":"Documents","groupLabel":null,"changeAction":null,"transliterate":false,"templateName":null,"fieldLayout":null,"locationHierarchy":null,"conditionalBioAttributes":null,"required":false,"bioAttributes":null,"requiredOn":[],"subType":"POE"}],"layoutTemplate":null,"preRegFetchRequired":false,"additionalInfoRequestIdRequired":true,"active":false}],"caption":{"eng":"Biometric correction","ara":"التصحيح البيومتري","fra":"Correction biométrique"},"icon":"UINUpdate.png","isActive":true,"autoSelectedGroups":null} </t>
+  </si>
+  <si>
+    <t>Pre-registration UI Specification</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -228,13 +215,12 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -273,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -281,25 +267,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,19 +491,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.5703125" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
     <col min="7" max="7" width="45.85546875" customWidth="1"/>
@@ -596,524 +573,524 @@
       </c>
     </row>
     <row r="2" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>18</v>
+      <c r="A2" s="6" t="s">
+        <v>24</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="6">
         <v>0.1</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>19</v>
+      <c r="C2" s="6" t="s">
+        <v>25</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>20</v>
+      <c r="D2" s="6" t="s">
+        <v>26</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>21</v>
+      <c r="E2" s="6" t="s">
+        <v>27</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>22</v>
+      <c r="F2" s="6" t="s">
+        <v>28</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>61</v>
+      <c r="G2" s="6" t="s">
+        <v>38</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="6">
         <v>1001</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="6">
         <v>0.1</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="6">
+        <v>110024</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="6">
+        <v>110005</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>24</v>
+      <c r="R2" s="6"/>
+    </row>
+    <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>32</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="B3" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" s="2"/>
-    </row>
-    <row r="3" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="2">
+      <c r="E3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="6">
         <v>1001</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="6">
         <v>0.1</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="6">
+        <v>110005</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="6">
+        <v>110005</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>24</v>
+      <c r="R3" s="6"/>
+    </row>
+    <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>29</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="B4" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>34</v>
+      <c r="D4" s="6" t="s">
+        <v>30</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>23</v>
+      <c r="E4" s="6" t="s">
+        <v>30</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>35</v>
+      <c r="F4" s="6" t="s">
+        <v>31</v>
       </c>
-      <c r="P3" s="2" t="s">
-        <v>23</v>
+      <c r="G4" s="6" t="s">
+        <v>40</v>
       </c>
-      <c r="Q3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R3" s="2"/>
-    </row>
-    <row r="4" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="2">
+      <c r="H4" s="6">
         <v>1001</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="6">
         <v>0.1</v>
       </c>
       <c r="J4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="6">
+        <v>110005</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="6">
+        <v>110005</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>24</v>
+      <c r="R4" s="6"/>
+    </row>
+    <row r="5" spans="1:26" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>41</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R4" s="2"/>
-    </row>
-    <row r="5" spans="1:26" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="B5" s="6">
         <v>0.1</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>29</v>
+      <c r="C5" s="6" t="s">
+        <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>41</v>
+      <c r="D5" s="6" t="s">
+        <v>57</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>22</v>
+      <c r="F5" s="6" t="s">
+        <v>19</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="6">
         <v>1001</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="6">
         <v>0.1</v>
       </c>
       <c r="J5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>24</v>
+      <c r="R5" s="6"/>
+    </row>
+    <row r="6" spans="1:26" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>45</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="B6" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="D6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1001</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="6">
+        <v>110024</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" s="6">
+        <v>110024</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R6" s="6"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+    </row>
+    <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="G7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="6">
+        <v>1001</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="6">
+        <v>110024</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" s="6">
+        <v>110024</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>35</v>
+      <c r="R7" s="6"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+    </row>
+    <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>51</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="B8" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="6">
+        <v>1001</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="6">
+        <v>110024</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" s="6">
+        <v>110024</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Q5" s="2" t="s">
-        <v>27</v>
+      <c r="R8" s="6"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+    </row>
+    <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>54</v>
       </c>
-      <c r="R5" s="6"/>
-    </row>
-    <row r="6" spans="1:26" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="7">
+      <c r="B9" s="6">
         <v>0.1</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>29</v>
+      <c r="C9" s="6" t="s">
+        <v>25</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>45</v>
+      <c r="D9" s="6" t="s">
+        <v>55</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>45</v>
+      <c r="E9" s="6" t="s">
+        <v>55</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>46</v>
+      <c r="F9" s="6" t="s">
+        <v>37</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>47</v>
+      <c r="G9" s="6" t="s">
+        <v>56</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H9" s="6">
         <v>1001</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I9" s="6">
         <v>0.1</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="6">
+        <v>110024</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O9" s="6">
+        <v>110024</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="R6" s="7"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8"/>
-      <c r="Z6" s="8"/>
-    </row>
-    <row r="7" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" s="7">
-        <v>1001</v>
-      </c>
-      <c r="I7" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="P7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="R7" s="7"/>
-      <c r="S7" s="8"/>
-      <c r="T7" s="8"/>
-      <c r="U7" s="8"/>
-      <c r="V7" s="8"/>
-      <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="8"/>
-      <c r="Z7" s="8"/>
-    </row>
-    <row r="8" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="7">
-        <v>1001</v>
-      </c>
-      <c r="I8" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="O8" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q8" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="R8" s="7"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="8"/>
-    </row>
-    <row r="9" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="7">
-        <v>1001</v>
-      </c>
-      <c r="I9" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="P9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="R9" s="7"/>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
-      <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
-      <c r="Z9" s="8"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="8"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="8"/>
-      <c r="V10" s="8"/>
-      <c r="W10" s="8"/>
-      <c r="X10" s="8"/>
-      <c r="Y10" s="8"/>
-      <c r="Z10" s="8"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="8"/>
-      <c r="T11" s="8"/>
-      <c r="U11" s="8"/>
-      <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="8"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -1122,7 +1099,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="9"/>
+      <c r="G12" s="5"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1142,7 +1119,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="9"/>
+      <c r="G13" s="5"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>

</xml_diff>